<commit_message>
fix typo name model
</commit_message>
<xml_diff>
--- a/Experiment_results/xlsx_format/ex_multi.xlsx
+++ b/Experiment_results/xlsx_format/ex_multi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\ДИПЛОМНЫЙ проект\результаты экспериментов\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A20392-E5AA-4ABB-863F-CDF2A1813DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D225208-0D24-44ED-86D5-4E5C98C38E22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1140,9 +1140,6 @@
     <t>PatchTST</t>
   </si>
   <si>
-    <t>SparseTFT</t>
-  </si>
-  <si>
     <t>0.383</t>
   </si>
   <si>
@@ -1309,6 +1306,9 @@
   </si>
   <si>
     <t>GTT-Tiny (finetune)</t>
+  </si>
+  <si>
+    <t>SparseTSF</t>
   </si>
 </sst>
 </file>
@@ -1629,8 +1629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6080771B-968D-4139-AF07-E0D46FA87262}">
   <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
-      <selection activeCell="P66" sqref="P66"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1659,22 +1659,22 @@
         <v>98</v>
       </c>
       <c r="D1" t="s">
+        <v>421</v>
+      </c>
+      <c r="E1" t="s">
+        <v>420</v>
+      </c>
+      <c r="F1" t="s">
         <v>422</v>
       </c>
-      <c r="E1" t="s">
-        <v>421</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>423</v>
-      </c>
-      <c r="G1" t="s">
-        <v>424</v>
       </c>
       <c r="H1" t="s">
         <v>313</v>
       </c>
       <c r="I1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="J1" t="s">
         <v>367</v>
@@ -1683,7 +1683,7 @@
         <v>358</v>
       </c>
       <c r="L1" t="s">
-        <v>368</v>
+        <v>424</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -1797,7 +1797,7 @@
         <v>43</v>
       </c>
       <c r="L4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1832,7 +1832,7 @@
         <v>191</v>
       </c>
       <c r="K5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="L5" t="s">
         <v>165</v>
@@ -2060,7 +2060,7 @@
         <v>194</v>
       </c>
       <c r="K11" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="L11" t="s">
         <v>165</v>
@@ -2177,7 +2177,7 @@
         <v>126</v>
       </c>
       <c r="L14" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -2212,7 +2212,7 @@
         <v>12</v>
       </c>
       <c r="K15" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="L15" t="s">
         <v>23</v>
@@ -2288,10 +2288,10 @@
         <v>144</v>
       </c>
       <c r="K17" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="L17" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -2326,10 +2326,10 @@
         <v>175</v>
       </c>
       <c r="K18" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="L18" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -2364,7 +2364,7 @@
         <v>182</v>
       </c>
       <c r="K19" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="L19" t="s">
         <v>266</v>
@@ -2405,7 +2405,7 @@
         <v>267</v>
       </c>
       <c r="L20" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
@@ -2478,10 +2478,10 @@
         <v>178</v>
       </c>
       <c r="K22" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="L22" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -2592,7 +2592,7 @@
         <v>200</v>
       </c>
       <c r="K25" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="L25" t="s">
         <v>207</v>
@@ -2630,10 +2630,10 @@
         <v>201</v>
       </c>
       <c r="K26" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="L26" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
@@ -2668,7 +2668,7 @@
         <v>146</v>
       </c>
       <c r="K27" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="L27" t="s">
         <v>265</v>
@@ -2706,7 +2706,7 @@
         <v>202</v>
       </c>
       <c r="K28" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="L28" t="s">
         <v>320</v>
@@ -2820,7 +2820,7 @@
         <v>107</v>
       </c>
       <c r="K31" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="L31" t="s">
         <v>208</v>
@@ -2861,7 +2861,7 @@
         <v>359</v>
       </c>
       <c r="L32" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
@@ -2899,7 +2899,7 @@
         <v>360</v>
       </c>
       <c r="L33" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
@@ -2937,7 +2937,7 @@
         <v>361</v>
       </c>
       <c r="L34" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
@@ -2975,7 +2975,7 @@
         <v>362</v>
       </c>
       <c r="L35" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
@@ -3010,10 +3010,10 @@
         <v>84</v>
       </c>
       <c r="K36" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="L36" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
@@ -3086,10 +3086,10 @@
         <v>27</v>
       </c>
       <c r="K38" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="L38" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
@@ -3124,7 +3124,7 @@
         <v>206</v>
       </c>
       <c r="K39" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="L39" t="s">
         <v>284</v>
@@ -3200,7 +3200,7 @@
         <v>128</v>
       </c>
       <c r="K41" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="L41" t="s">
         <v>202</v>
@@ -3431,7 +3431,7 @@
         <v>21</v>
       </c>
       <c r="L47" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
@@ -3466,7 +3466,7 @@
         <v>153</v>
       </c>
       <c r="K48" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="L48" t="s">
         <v>168</v>
@@ -3504,7 +3504,7 @@
         <v>209</v>
       </c>
       <c r="K49" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L49" t="s">
         <v>47</v>
@@ -3545,7 +3545,7 @@
         <v>206</v>
       </c>
       <c r="L50" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
@@ -3580,7 +3580,7 @@
         <v>211</v>
       </c>
       <c r="K51" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="L51" t="s">
         <v>108</v>
@@ -3618,10 +3618,10 @@
         <v>212</v>
       </c>
       <c r="K52" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="L52" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
@@ -3656,7 +3656,7 @@
         <v>213</v>
       </c>
       <c r="K53" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="L53" t="s">
         <v>129</v>
@@ -3770,10 +3770,10 @@
         <v>109</v>
       </c>
       <c r="K56" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="L56" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
@@ -3808,10 +3808,10 @@
         <v>214</v>
       </c>
       <c r="K57" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="L57" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
@@ -3846,10 +3846,10 @@
         <v>202</v>
       </c>
       <c r="K58" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="L58" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
@@ -3884,7 +3884,7 @@
         <v>126</v>
       </c>
       <c r="K59" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="L59" t="s">
         <v>156</v>
@@ -3922,10 +3922,10 @@
         <v>215</v>
       </c>
       <c r="K60" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L60" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
@@ -3960,10 +3960,10 @@
         <v>91</v>
       </c>
       <c r="K61" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L61" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
@@ -3998,10 +3998,10 @@
         <v>216</v>
       </c>
       <c r="K62" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="L62" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
@@ -4036,7 +4036,7 @@
         <v>181</v>
       </c>
       <c r="K63" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="L63" t="s">
         <v>148</v>
@@ -4077,7 +4077,7 @@
         <v>117</v>
       </c>
       <c r="L64" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
@@ -4153,7 +4153,7 @@
         <v>363</v>
       </c>
       <c r="L66" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
@@ -4191,7 +4191,7 @@
         <v>364</v>
       </c>
       <c r="L67" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
@@ -4229,7 +4229,7 @@
         <v>365</v>
       </c>
       <c r="L68" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
@@ -4267,7 +4267,7 @@
         <v>366</v>
       </c>
       <c r="L69" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new table and full update
</commit_message>
<xml_diff>
--- a/Experiment_results/xlsx_format/ex_multi.xlsx
+++ b/Experiment_results/xlsx_format/ex_multi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\ДИПЛОМНЫЙ проект\результаты экспериментов\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4155C000-0365-45E8-A295-D204840FD99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B923ACB-41BE-4A88-9707-3495A1EB6DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="571">
   <si>
     <t>ETTh1</t>
   </si>
@@ -1306,6 +1306,447 @@
   </si>
   <si>
     <t>SparseTSF</t>
+  </si>
+  <si>
+    <t>ModernTCN</t>
+  </si>
+  <si>
+    <t>0.290</t>
+  </si>
+  <si>
+    <t>0.257</t>
+  </si>
+  <si>
+    <t>0.103</t>
+  </si>
+  <si>
+    <t>0.197</t>
+  </si>
+  <si>
+    <t>0.583</t>
+  </si>
+  <si>
+    <t>0.718</t>
+  </si>
+  <si>
+    <t>0.819</t>
+  </si>
+  <si>
+    <t>0.781</t>
+  </si>
+  <si>
+    <t>0.157</t>
+  </si>
+  <si>
+    <t>0.081</t>
+  </si>
+  <si>
+    <t>0.659</t>
+  </si>
+  <si>
+    <t>1.348</t>
+  </si>
+  <si>
+    <t>1.446</t>
+  </si>
+  <si>
+    <t>1.389</t>
+  </si>
+  <si>
+    <t>1.773</t>
+  </si>
+  <si>
+    <t>0.671</t>
+  </si>
+  <si>
+    <t>0.476</t>
+  </si>
+  <si>
+    <t>0.733</t>
+  </si>
+  <si>
+    <t>0.746</t>
+  </si>
+  <si>
+    <t>0.473</t>
+  </si>
+  <si>
+    <t>0.690</t>
+  </si>
+  <si>
+    <t>0.289</t>
+  </si>
+  <si>
+    <t>0.713</t>
+  </si>
+  <si>
+    <t>0.720</t>
+  </si>
+  <si>
+    <t>0.665</t>
+  </si>
+  <si>
+    <t>0.136</t>
+  </si>
+  <si>
+    <t>0.511</t>
+  </si>
+  <si>
+    <t>0.677</t>
+  </si>
+  <si>
+    <t>0.707</t>
+  </si>
+  <si>
+    <t>0.730</t>
+  </si>
+  <si>
+    <t>6.213</t>
+  </si>
+  <si>
+    <t>7.714</t>
+  </si>
+  <si>
+    <t>7.851</t>
+  </si>
+  <si>
+    <t>6.885</t>
+  </si>
+  <si>
+    <t>1.622</t>
+  </si>
+  <si>
+    <t>1.906</t>
+  </si>
+  <si>
+    <t>1.952</t>
+  </si>
+  <si>
+    <t>1.788</t>
+  </si>
+  <si>
+    <t>1.222</t>
+  </si>
+  <si>
+    <t>0.149</t>
+  </si>
+  <si>
+    <t>1.294</t>
+  </si>
+  <si>
+    <t>1.214</t>
+  </si>
+  <si>
+    <t>0.259</t>
+  </si>
+  <si>
+    <t>1.325</t>
+  </si>
+  <si>
+    <t>0.534</t>
+  </si>
+  <si>
+    <t>1.261</t>
+  </si>
+  <si>
+    <t>0.309</t>
+  </si>
+  <si>
+    <t>1.330</t>
+  </si>
+  <si>
+    <t>0.597</t>
+  </si>
+  <si>
+    <t>1.287</t>
+  </si>
+  <si>
+    <t>0.306</t>
+  </si>
+  <si>
+    <t>1.335</t>
+  </si>
+  <si>
+    <t>0.595</t>
+  </si>
+  <si>
+    <t>1.322</t>
+  </si>
+  <si>
+    <t>0.810</t>
+  </si>
+  <si>
+    <t>0.129</t>
+  </si>
+  <si>
+    <t>0.204</t>
+  </si>
+  <si>
+    <t>0.236</t>
+  </si>
+  <si>
+    <t>de_small</t>
+  </si>
+  <si>
+    <t>de_big</t>
+  </si>
+  <si>
+    <t>0.288</t>
+  </si>
+  <si>
+    <t>0.151</t>
+  </si>
+  <si>
+    <t>0.146</t>
+  </si>
+  <si>
+    <t>0.463</t>
+  </si>
+  <si>
+    <t>0.612</t>
+  </si>
+  <si>
+    <t>0.227</t>
+  </si>
+  <si>
+    <t>0.488</t>
+  </si>
+  <si>
+    <t>0.562</t>
+  </si>
+  <si>
+    <t>0.706</t>
+  </si>
+  <si>
+    <t>0.068</t>
+  </si>
+  <si>
+    <t>0.284</t>
+  </si>
+  <si>
+    <t>0.451</t>
+  </si>
+  <si>
+    <t>0.515</t>
+  </si>
+  <si>
+    <t>0.541</t>
+  </si>
+  <si>
+    <t>0.577</t>
+  </si>
+  <si>
+    <t>0.513</t>
+  </si>
+  <si>
+    <t>0.565</t>
+  </si>
+  <si>
+    <t>0.078</t>
+  </si>
+  <si>
+    <t>0.127</t>
+  </si>
+  <si>
+    <t>0.211</t>
+  </si>
+  <si>
+    <t>0.261</t>
+  </si>
+  <si>
+    <t>0.295</t>
+  </si>
+  <si>
+    <t>0.228</t>
+  </si>
+  <si>
+    <t>0.180</t>
+  </si>
+  <si>
+    <t>0.926</t>
+  </si>
+  <si>
+    <t>0.924</t>
+  </si>
+  <si>
+    <t>0.903</t>
+  </si>
+  <si>
+    <t>0.913</t>
+  </si>
+  <si>
+    <t>0.948</t>
+  </si>
+  <si>
+    <t>0.981</t>
+  </si>
+  <si>
+    <t>1.033</t>
+  </si>
+  <si>
+    <t>1.011</t>
+  </si>
+  <si>
+    <t>1.012</t>
+  </si>
+  <si>
+    <t>1.367</t>
+  </si>
+  <si>
+    <t>1.436</t>
+  </si>
+  <si>
+    <t>1.163</t>
+  </si>
+  <si>
+    <t>1.192</t>
+  </si>
+  <si>
+    <t>1.141</t>
+  </si>
+  <si>
+    <t>1.179</t>
+  </si>
+  <si>
+    <t>1.290</t>
+  </si>
+  <si>
+    <t>0.440</t>
+  </si>
+  <si>
+    <t>0.553</t>
+  </si>
+  <si>
+    <t>0.603</t>
+  </si>
+  <si>
+    <t>0.245</t>
+  </si>
+  <si>
+    <t>0.283</t>
+  </si>
+  <si>
+    <t>0.542</t>
+  </si>
+  <si>
+    <t>0.634</t>
+  </si>
+  <si>
+    <t>0.123</t>
+  </si>
+  <si>
+    <t>0.173</t>
+  </si>
+  <si>
+    <t>0.066</t>
+  </si>
+  <si>
+    <t>0.075</t>
+  </si>
+  <si>
+    <t>0.895</t>
+  </si>
+  <si>
+    <t>1.068</t>
+  </si>
+  <si>
+    <t>1.056</t>
+  </si>
+  <si>
+    <t>1.093</t>
+  </si>
+  <si>
+    <t>1.124</t>
+  </si>
+  <si>
+    <t>1.065</t>
+  </si>
+  <si>
+    <t>1.067</t>
+  </si>
+  <si>
+    <t>1.111</t>
+  </si>
+  <si>
+    <t>1.636</t>
+  </si>
+  <si>
+    <t>1.846</t>
+  </si>
+  <si>
+    <t>1.838</t>
+  </si>
+  <si>
+    <t>1.976</t>
+  </si>
+  <si>
+    <t>1.304</t>
+  </si>
+  <si>
+    <t>1.757</t>
+  </si>
+  <si>
+    <t>1.724</t>
+  </si>
+  <si>
+    <t>1.834</t>
+  </si>
+  <si>
+    <t>1.937</t>
+  </si>
+  <si>
+    <t>0.389</t>
+  </si>
+  <si>
+    <t>0.334</t>
+  </si>
+  <si>
+    <t>0.102</t>
+  </si>
+  <si>
+    <t>0.171</t>
+  </si>
+  <si>
+    <t>0.235</t>
+  </si>
+  <si>
+    <t>0.160</t>
+  </si>
+  <si>
+    <t>0.125</t>
+  </si>
+  <si>
+    <t>0.524</t>
+  </si>
+  <si>
+    <t>0.520</t>
+  </si>
+  <si>
+    <t>0.503</t>
+  </si>
+  <si>
+    <t>0.481</t>
+  </si>
+  <si>
+    <t>0.138</t>
+  </si>
+  <si>
+    <t>0.055</t>
+  </si>
+  <si>
+    <t>0.174</t>
+  </si>
+  <si>
+    <t>0.132</t>
+  </si>
+  <si>
+    <t>0.268</t>
+  </si>
+  <si>
+    <t>0.048</t>
+  </si>
+  <si>
+    <t>Repeat_Closest</t>
   </si>
 </sst>
 </file>
@@ -1624,10 +2065,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6080771B-968D-4139-AF07-E0D46FA87262}">
-  <dimension ref="A1:L69"/>
+  <dimension ref="A1:N87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M32" sqref="M32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1643,9 +2084,11 @@
     <col min="10" max="10" width="9.6640625" customWidth="1"/>
     <col min="11" max="11" width="9.109375" customWidth="1"/>
     <col min="12" max="12" width="9.44140625" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" customWidth="1"/>
+    <col min="14" max="14" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>96</v>
       </c>
@@ -1682,8 +2125,14 @@
       <c r="L1" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M1" t="s">
+        <v>424</v>
+      </c>
+      <c r="N1" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>24</v>
       </c>
@@ -1720,8 +2169,14 @@
       <c r="L2" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M2" t="s">
+        <v>125</v>
+      </c>
+      <c r="N2" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>96</v>
       </c>
@@ -1758,8 +2213,14 @@
       <c r="L3" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M3" t="s">
+        <v>245</v>
+      </c>
+      <c r="N3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>192</v>
       </c>
@@ -1796,8 +2257,14 @@
       <c r="L4" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>336</v>
       </c>
@@ -1834,8 +2301,14 @@
       <c r="L5" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5" t="s">
+        <v>370</v>
+      </c>
+      <c r="N5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>720</v>
       </c>
@@ -1872,8 +2345,14 @@
       <c r="L6" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M6" t="s">
+        <v>165</v>
+      </c>
+      <c r="N6" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>24</v>
       </c>
@@ -1910,8 +2389,14 @@
       <c r="L7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M7" t="s">
+        <v>426</v>
+      </c>
+      <c r="N7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>96</v>
       </c>
@@ -1948,8 +2433,14 @@
       <c r="L8" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M8" t="s">
+        <v>121</v>
+      </c>
+      <c r="N8" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>192</v>
       </c>
@@ -1986,8 +2477,14 @@
       <c r="L9" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M9" t="s">
+        <v>258</v>
+      </c>
+      <c r="N9" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>336</v>
       </c>
@@ -2024,8 +2521,14 @@
       <c r="L10" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M10" t="s">
+        <v>149</v>
+      </c>
+      <c r="N10" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>720</v>
       </c>
@@ -2062,8 +2565,14 @@
       <c r="L11" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M11" t="s">
+        <v>115</v>
+      </c>
+      <c r="N11" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>24</v>
       </c>
@@ -2100,8 +2609,14 @@
       <c r="L12" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M12" t="s">
+        <v>495</v>
+      </c>
+      <c r="N12" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>96</v>
       </c>
@@ -2138,8 +2653,14 @@
       <c r="L13" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M13" t="s">
+        <v>384</v>
+      </c>
+      <c r="N13" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>192</v>
       </c>
@@ -2176,8 +2697,14 @@
       <c r="L14" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M14" t="s">
+        <v>125</v>
+      </c>
+      <c r="N14" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>336</v>
       </c>
@@ -2214,8 +2741,14 @@
       <c r="L15" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M15" t="s">
+        <v>245</v>
+      </c>
+      <c r="N15" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>720</v>
       </c>
@@ -2252,8 +2785,14 @@
       <c r="L16" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M16" t="s">
+        <v>36</v>
+      </c>
+      <c r="N16" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>24</v>
       </c>
@@ -2290,8 +2829,14 @@
       <c r="L17" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M17" t="s">
+        <v>396</v>
+      </c>
+      <c r="N17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>96</v>
       </c>
@@ -2328,8 +2873,14 @@
       <c r="L18" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M18" t="s">
+        <v>467</v>
+      </c>
+      <c r="N18" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>192</v>
       </c>
@@ -2366,8 +2917,14 @@
       <c r="L19" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M19" t="s">
+        <v>109</v>
+      </c>
+      <c r="N19" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>336</v>
       </c>
@@ -2404,8 +2961,14 @@
       <c r="L20" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M20" t="s">
+        <v>196</v>
+      </c>
+      <c r="N20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>720</v>
       </c>
@@ -2442,8 +3005,14 @@
       <c r="L21" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M21" t="s">
+        <v>553</v>
+      </c>
+      <c r="N21" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>24</v>
       </c>
@@ -2480,8 +3049,14 @@
       <c r="L22" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M22" t="s">
+        <v>427</v>
+      </c>
+      <c r="N22" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>96</v>
       </c>
@@ -2518,8 +3093,14 @@
       <c r="L23" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M23" t="s">
+        <v>428</v>
+      </c>
+      <c r="N23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>192</v>
       </c>
@@ -2556,8 +3137,14 @@
       <c r="L24" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M24" t="s">
+        <v>425</v>
+      </c>
+      <c r="N24" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>336</v>
       </c>
@@ -2594,8 +3181,14 @@
       <c r="L25" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M25" t="s">
+        <v>223</v>
+      </c>
+      <c r="N25" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>720</v>
       </c>
@@ -2632,8 +3225,14 @@
       <c r="L26" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M26" t="s">
+        <v>429</v>
+      </c>
+      <c r="N26" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>24</v>
       </c>
@@ -2670,8 +3269,14 @@
       <c r="L27" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M27" t="s">
+        <v>480</v>
+      </c>
+      <c r="N27" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>96</v>
       </c>
@@ -2708,8 +3313,14 @@
       <c r="L28" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M28" t="s">
+        <v>481</v>
+      </c>
+      <c r="N28" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>192</v>
       </c>
@@ -2746,8 +3357,14 @@
       <c r="L29" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M29" t="s">
+        <v>13</v>
+      </c>
+      <c r="N29" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>336</v>
       </c>
@@ -2784,8 +3401,14 @@
       <c r="L30" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M30" t="s">
+        <v>184</v>
+      </c>
+      <c r="N30" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>720</v>
       </c>
@@ -2822,8 +3445,14 @@
       <c r="L31" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M31" t="s">
+        <v>139</v>
+      </c>
+      <c r="N31" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>24</v>
       </c>
@@ -2860,8 +3489,14 @@
       <c r="L32" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M32" t="s">
+        <v>430</v>
+      </c>
+      <c r="N32" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>36</v>
       </c>
@@ -2898,8 +3533,14 @@
       <c r="L33" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M33" t="s">
+        <v>431</v>
+      </c>
+      <c r="N33" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>48</v>
       </c>
@@ -2936,8 +3577,14 @@
       <c r="L34" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M34" t="s">
+        <v>432</v>
+      </c>
+      <c r="N34" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>60</v>
       </c>
@@ -2974,1297 +3621,2299 @@
       <c r="L35" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M35" t="s">
+        <v>204</v>
+      </c>
+      <c r="N35" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>24</v>
       </c>
       <c r="B36" t="s">
-        <v>0</v>
+        <v>483</v>
       </c>
       <c r="C36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D36" t="s">
-        <v>51</v>
+        <v>250</v>
       </c>
       <c r="E36" t="s">
-        <v>144</v>
+        <v>266</v>
       </c>
       <c r="F36" t="s">
-        <v>109</v>
+        <v>233</v>
       </c>
       <c r="G36" t="s">
-        <v>181</v>
+        <v>560</v>
       </c>
       <c r="H36" t="s">
-        <v>336</v>
+        <v>514</v>
       </c>
       <c r="I36" t="s">
-        <v>72</v>
+        <v>525</v>
       </c>
       <c r="J36" t="s">
-        <v>83</v>
+        <v>329</v>
       </c>
       <c r="K36" t="s">
-        <v>383</v>
+        <v>79</v>
       </c>
       <c r="L36" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+        <v>496</v>
+      </c>
+      <c r="M36" t="s">
+        <v>398</v>
+      </c>
+      <c r="N36" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>483</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" t="s">
+        <v>117</v>
+      </c>
+      <c r="E37" t="s">
+        <v>195</v>
+      </c>
+      <c r="F37" t="s">
+        <v>148</v>
+      </c>
+      <c r="G37" t="s">
+        <v>561</v>
+      </c>
+      <c r="H37" t="s">
+        <v>517</v>
+      </c>
+      <c r="I37" t="s">
+        <v>497</v>
+      </c>
+      <c r="J37" t="s">
+        <v>54</v>
+      </c>
+      <c r="K37" t="s">
+        <v>488</v>
+      </c>
+      <c r="L37" t="s">
+        <v>497</v>
+      </c>
+      <c r="M37" t="s">
+        <v>485</v>
+      </c>
+      <c r="N37" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>48</v>
+      </c>
+      <c r="B38" t="s">
+        <v>483</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" t="s">
+        <v>382</v>
+      </c>
+      <c r="E38" t="s">
+        <v>192</v>
+      </c>
+      <c r="F38" t="s">
+        <v>84</v>
+      </c>
+      <c r="G38" t="s">
+        <v>562</v>
+      </c>
+      <c r="H38" t="s">
+        <v>516</v>
+      </c>
+      <c r="I38" t="s">
+        <v>526</v>
+      </c>
+      <c r="J38" t="s">
+        <v>12</v>
+      </c>
+      <c r="K38" t="s">
+        <v>286</v>
+      </c>
+      <c r="L38" t="s">
+        <v>498</v>
+      </c>
+      <c r="M38" t="s">
+        <v>139</v>
+      </c>
+      <c r="N38" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>60</v>
+      </c>
+      <c r="B39" t="s">
+        <v>483</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" t="s">
+        <v>41</v>
+      </c>
+      <c r="E39" t="s">
+        <v>149</v>
+      </c>
+      <c r="F39" t="s">
+        <v>42</v>
+      </c>
+      <c r="G39" t="s">
+        <v>563</v>
+      </c>
+      <c r="H39" t="s">
+        <v>515</v>
+      </c>
+      <c r="I39" t="s">
+        <v>527</v>
+      </c>
+      <c r="J39" t="s">
+        <v>116</v>
+      </c>
+      <c r="K39" t="s">
+        <v>489</v>
+      </c>
+      <c r="L39" t="s">
+        <v>499</v>
+      </c>
+      <c r="M39" t="s">
+        <v>265</v>
+      </c>
+      <c r="N39" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>24</v>
+      </c>
+      <c r="B40" t="s">
+        <v>484</v>
+      </c>
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" t="s">
+        <v>389</v>
+      </c>
+      <c r="E40" t="s">
+        <v>567</v>
+      </c>
+      <c r="F40" t="s">
+        <v>399</v>
+      </c>
+      <c r="G40" t="s">
+        <v>564</v>
+      </c>
+      <c r="H40" t="s">
+        <v>509</v>
+      </c>
+      <c r="I40" t="s">
+        <v>528</v>
+      </c>
+      <c r="J40" t="s">
+        <v>390</v>
+      </c>
+      <c r="K40" t="s">
+        <v>385</v>
+      </c>
+      <c r="L40" t="s">
+        <v>160</v>
+      </c>
+      <c r="M40" t="s">
+        <v>371</v>
+      </c>
+      <c r="N40" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A41">
         <v>96</v>
       </c>
-      <c r="B37" t="s">
-        <v>0</v>
-      </c>
-      <c r="C37" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" t="s">
-        <v>149</v>
-      </c>
-      <c r="E37" t="s">
-        <v>93</v>
-      </c>
-      <c r="F37" t="s">
-        <v>241</v>
-      </c>
-      <c r="G37" t="s">
-        <v>163</v>
-      </c>
-      <c r="H37" t="s">
-        <v>337</v>
-      </c>
-      <c r="I37" t="s">
-        <v>73</v>
-      </c>
-      <c r="J37" t="s">
-        <v>135</v>
-      </c>
-      <c r="K37" t="s">
-        <v>226</v>
-      </c>
-      <c r="L37" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38">
+      <c r="B41" t="s">
+        <v>484</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" t="s">
+        <v>557</v>
+      </c>
+      <c r="E41" t="s">
+        <v>18</v>
+      </c>
+      <c r="F41" t="s">
+        <v>490</v>
+      </c>
+      <c r="G41" t="s">
+        <v>329</v>
+      </c>
+      <c r="H41" t="s">
+        <v>510</v>
+      </c>
+      <c r="I41" t="s">
+        <v>529</v>
+      </c>
+      <c r="J41" t="s">
+        <v>19</v>
+      </c>
+      <c r="K41" t="s">
+        <v>490</v>
+      </c>
+      <c r="L41" t="s">
+        <v>170</v>
+      </c>
+      <c r="M41" t="s">
+        <v>426</v>
+      </c>
+      <c r="N41" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A42">
         <v>192</v>
       </c>
-      <c r="B38" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" t="s">
-        <v>283</v>
-      </c>
-      <c r="E38" t="s">
-        <v>114</v>
-      </c>
-      <c r="F38" t="s">
-        <v>115</v>
-      </c>
-      <c r="G38" t="s">
-        <v>164</v>
-      </c>
-      <c r="H38" t="s">
-        <v>338</v>
-      </c>
-      <c r="I38" t="s">
-        <v>74</v>
-      </c>
-      <c r="J38" t="s">
-        <v>26</v>
-      </c>
-      <c r="K38" t="s">
-        <v>367</v>
-      </c>
-      <c r="L38" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <v>336</v>
-      </c>
-      <c r="B39" t="s">
-        <v>0</v>
-      </c>
-      <c r="C39" t="s">
-        <v>8</v>
-      </c>
-      <c r="D39" t="s">
-        <v>89</v>
-      </c>
-      <c r="E39" t="s">
-        <v>132</v>
-      </c>
-      <c r="F39" t="s">
-        <v>165</v>
-      </c>
-      <c r="G39" t="s">
-        <v>262</v>
-      </c>
-      <c r="H39" t="s">
-        <v>339</v>
-      </c>
-      <c r="I39" t="s">
-        <v>75</v>
-      </c>
-      <c r="J39" t="s">
-        <v>205</v>
-      </c>
-      <c r="K39" t="s">
-        <v>374</v>
-      </c>
-      <c r="L39" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A40">
-        <v>720</v>
-      </c>
-      <c r="B40" t="s">
-        <v>0</v>
-      </c>
-      <c r="C40" t="s">
-        <v>8</v>
-      </c>
-      <c r="D40" t="s">
-        <v>284</v>
-      </c>
-      <c r="E40" t="s">
-        <v>304</v>
-      </c>
-      <c r="F40" t="s">
-        <v>242</v>
-      </c>
-      <c r="G40" t="s">
-        <v>263</v>
-      </c>
-      <c r="H40" t="s">
-        <v>340</v>
-      </c>
-      <c r="I40" t="s">
-        <v>76</v>
-      </c>
-      <c r="J40" t="s">
-        <v>206</v>
-      </c>
-      <c r="K40" t="s">
-        <v>234</v>
-      </c>
-      <c r="L40" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <v>24</v>
-      </c>
-      <c r="B41" t="s">
-        <v>1</v>
-      </c>
-      <c r="C41" t="s">
-        <v>8</v>
-      </c>
-      <c r="D41" t="s">
-        <v>133</v>
-      </c>
-      <c r="E41" t="s">
-        <v>23</v>
-      </c>
-      <c r="F41" t="s">
-        <v>243</v>
-      </c>
-      <c r="G41" t="s">
-        <v>264</v>
-      </c>
-      <c r="H41" t="s">
-        <v>143</v>
-      </c>
-      <c r="I41" t="s">
-        <v>77</v>
-      </c>
-      <c r="J41" t="s">
-        <v>127</v>
-      </c>
-      <c r="K41" t="s">
-        <v>385</v>
-      </c>
-      <c r="L41" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42">
-        <v>96</v>
-      </c>
       <c r="B42" t="s">
-        <v>1</v>
+        <v>484</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D42" t="s">
+        <v>276</v>
+      </c>
+      <c r="E42" t="s">
         <v>116</v>
       </c>
-      <c r="E42" t="s">
-        <v>212</v>
-      </c>
       <c r="F42" t="s">
-        <v>221</v>
+        <v>120</v>
       </c>
       <c r="G42" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="H42" t="s">
-        <v>341</v>
+        <v>511</v>
       </c>
       <c r="I42" t="s">
         <v>78</v>
       </c>
       <c r="J42" t="s">
-        <v>194</v>
+        <v>233</v>
       </c>
       <c r="K42" t="s">
-        <v>14</v>
+        <v>276</v>
       </c>
       <c r="L42" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+      <c r="M42" t="s">
+        <v>425</v>
+      </c>
+      <c r="N42" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43">
+        <v>336</v>
+      </c>
+      <c r="B43" t="s">
+        <v>484</v>
+      </c>
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" t="s">
+        <v>372</v>
+      </c>
+      <c r="E43" t="s">
+        <v>568</v>
+      </c>
+      <c r="F43" t="s">
+        <v>506</v>
+      </c>
+      <c r="G43" t="s">
+        <v>19</v>
+      </c>
+      <c r="H43" t="s">
+        <v>512</v>
+      </c>
+      <c r="I43" t="s">
+        <v>152</v>
+      </c>
+      <c r="J43" t="s">
+        <v>106</v>
+      </c>
+      <c r="K43" t="s">
+        <v>372</v>
+      </c>
+      <c r="L43" t="s">
+        <v>88</v>
+      </c>
+      <c r="M43" t="s">
+        <v>384</v>
+      </c>
+      <c r="N43" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>720</v>
+      </c>
+      <c r="B44" t="s">
+        <v>484</v>
+      </c>
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" t="s">
+        <v>48</v>
+      </c>
+      <c r="E44" t="s">
+        <v>341</v>
+      </c>
+      <c r="F44" t="s">
+        <v>266</v>
+      </c>
+      <c r="G44" t="s">
+        <v>171</v>
+      </c>
+      <c r="H44" t="s">
+        <v>513</v>
+      </c>
+      <c r="I44" t="s">
+        <v>11</v>
+      </c>
+      <c r="J44" t="s">
         <v>192</v>
       </c>
-      <c r="B43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C43" t="s">
-        <v>8</v>
-      </c>
-      <c r="D43" t="s">
-        <v>285</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="K44" t="s">
+        <v>155</v>
+      </c>
+      <c r="L44" t="s">
+        <v>93</v>
+      </c>
+      <c r="M44" t="s">
+        <v>73</v>
+      </c>
+      <c r="N44" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A45">
         <v>24</v>
       </c>
-      <c r="F43" t="s">
-        <v>136</v>
-      </c>
-      <c r="G43" t="s">
-        <v>227</v>
-      </c>
-      <c r="H43" t="s">
-        <v>244</v>
-      </c>
-      <c r="I43" t="s">
-        <v>79</v>
-      </c>
-      <c r="J43" t="s">
-        <v>207</v>
-      </c>
-      <c r="K43" t="s">
-        <v>198</v>
-      </c>
-      <c r="L43" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A44">
-        <v>336</v>
-      </c>
-      <c r="B44" t="s">
-        <v>1</v>
-      </c>
-      <c r="C44" t="s">
-        <v>8</v>
-      </c>
-      <c r="D44" t="s">
-        <v>167</v>
-      </c>
-      <c r="E44" t="s">
-        <v>233</v>
-      </c>
-      <c r="F44" t="s">
-        <v>88</v>
-      </c>
-      <c r="G44" t="s">
-        <v>142</v>
-      </c>
-      <c r="H44" t="s">
-        <v>36</v>
-      </c>
-      <c r="I44" t="s">
-        <v>80</v>
-      </c>
-      <c r="J44" t="s">
-        <v>152</v>
-      </c>
-      <c r="K44" t="s">
-        <v>121</v>
-      </c>
-      <c r="L44" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <v>720</v>
-      </c>
       <c r="B45" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C45" t="s">
         <v>8</v>
       </c>
       <c r="D45" t="s">
-        <v>225</v>
+        <v>51</v>
       </c>
       <c r="E45" t="s">
-        <v>258</v>
+        <v>144</v>
       </c>
       <c r="F45" t="s">
-        <v>244</v>
+        <v>109</v>
       </c>
       <c r="G45" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
       <c r="H45" t="s">
-        <v>44</v>
+        <v>336</v>
       </c>
       <c r="I45" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="J45" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="K45" t="s">
-        <v>352</v>
+        <v>383</v>
       </c>
       <c r="L45" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+        <v>401</v>
+      </c>
+      <c r="M45" t="s">
+        <v>162</v>
+      </c>
+      <c r="N45" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="B46" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C46" t="s">
         <v>8</v>
       </c>
       <c r="D46" t="s">
-        <v>184</v>
+        <v>149</v>
       </c>
       <c r="E46" t="s">
-        <v>146</v>
+        <v>93</v>
       </c>
       <c r="F46" t="s">
-        <v>147</v>
+        <v>241</v>
       </c>
       <c r="G46" t="s">
-        <v>99</v>
+        <v>163</v>
       </c>
       <c r="H46" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="I46" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="J46" t="s">
-        <v>34</v>
+        <v>135</v>
       </c>
       <c r="K46" t="s">
-        <v>169</v>
+        <v>226</v>
       </c>
       <c r="L46" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+      <c r="M46" t="s">
+        <v>195</v>
+      </c>
+      <c r="N46" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>96</v>
+        <v>192</v>
       </c>
       <c r="B47" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C47" t="s">
         <v>8</v>
       </c>
       <c r="D47" t="s">
-        <v>81</v>
+        <v>283</v>
       </c>
       <c r="E47" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="F47" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="G47" t="s">
-        <v>265</v>
+        <v>164</v>
       </c>
       <c r="H47" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="I47" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="J47" t="s">
-        <v>181</v>
+        <v>26</v>
       </c>
       <c r="K47" t="s">
-        <v>20</v>
+        <v>367</v>
       </c>
       <c r="L47" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+        <v>374</v>
+      </c>
+      <c r="M47" t="s">
+        <v>114</v>
+      </c>
+      <c r="N47" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>192</v>
+        <v>336</v>
       </c>
       <c r="B48" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C48" t="s">
         <v>8</v>
       </c>
       <c r="D48" t="s">
-        <v>286</v>
+        <v>89</v>
       </c>
       <c r="E48" t="s">
-        <v>196</v>
+        <v>132</v>
       </c>
       <c r="F48" t="s">
-        <v>245</v>
+        <v>165</v>
       </c>
       <c r="G48" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="H48" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="I48" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="J48" t="s">
-        <v>152</v>
+        <v>205</v>
       </c>
       <c r="K48" t="s">
-        <v>386</v>
+        <v>374</v>
       </c>
       <c r="L48" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+        <v>283</v>
+      </c>
+      <c r="M48" t="s">
+        <v>11</v>
+      </c>
+      <c r="N48" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>336</v>
+        <v>720</v>
       </c>
       <c r="B49" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C49" t="s">
         <v>8</v>
       </c>
       <c r="D49" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E49" t="s">
-        <v>46</v>
+        <v>304</v>
       </c>
       <c r="F49" t="s">
-        <v>225</v>
+        <v>242</v>
       </c>
       <c r="G49" t="s">
-        <v>84</v>
+        <v>263</v>
       </c>
       <c r="H49" t="s">
-        <v>271</v>
+        <v>340</v>
       </c>
       <c r="I49" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="J49" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="K49" t="s">
-        <v>387</v>
+        <v>234</v>
       </c>
       <c r="L49" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+      <c r="M49" t="s">
+        <v>206</v>
+      </c>
+      <c r="N49" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>720</v>
+        <v>24</v>
       </c>
       <c r="B50" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C50" t="s">
         <v>8</v>
       </c>
       <c r="D50" t="s">
-        <v>94</v>
+        <v>133</v>
       </c>
       <c r="E50" t="s">
-        <v>81</v>
+        <v>23</v>
       </c>
       <c r="F50" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="G50" t="s">
-        <v>225</v>
+        <v>264</v>
       </c>
       <c r="H50" t="s">
-        <v>249</v>
+        <v>143</v>
       </c>
       <c r="I50" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="J50" t="s">
-        <v>209</v>
+        <v>127</v>
       </c>
       <c r="K50" t="s">
-        <v>205</v>
+        <v>385</v>
       </c>
       <c r="L50" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+      <c r="M50" t="s">
+        <v>433</v>
+      </c>
+      <c r="N50" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="B51" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C51" t="s">
         <v>8</v>
       </c>
       <c r="D51" t="s">
-        <v>288</v>
+        <v>116</v>
       </c>
       <c r="E51" t="s">
-        <v>32</v>
+        <v>212</v>
       </c>
       <c r="F51" t="s">
-        <v>68</v>
+        <v>221</v>
       </c>
       <c r="G51" t="s">
-        <v>16</v>
+        <v>104</v>
       </c>
       <c r="H51" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="I51" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="J51" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="K51" t="s">
-        <v>388</v>
+        <v>14</v>
       </c>
       <c r="L51" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="M51" t="s">
+        <v>138</v>
+      </c>
+      <c r="N51" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>96</v>
+        <v>192</v>
       </c>
       <c r="B52" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C52" t="s">
         <v>8</v>
       </c>
       <c r="D52" t="s">
-        <v>201</v>
+        <v>285</v>
       </c>
       <c r="E52" t="s">
-        <v>305</v>
+        <v>24</v>
       </c>
       <c r="F52" t="s">
-        <v>179</v>
+        <v>136</v>
       </c>
       <c r="G52" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="H52" t="s">
-        <v>12</v>
+        <v>244</v>
       </c>
       <c r="I52" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J52" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="K52" t="s">
-        <v>389</v>
+        <v>198</v>
       </c>
       <c r="L52" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="M52" t="s">
+        <v>401</v>
+      </c>
+      <c r="N52" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>192</v>
+        <v>336</v>
       </c>
       <c r="B53" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C53" t="s">
         <v>8</v>
       </c>
       <c r="D53" t="s">
-        <v>105</v>
+        <v>167</v>
       </c>
       <c r="E53" t="s">
-        <v>137</v>
+        <v>233</v>
       </c>
       <c r="F53" t="s">
-        <v>194</v>
+        <v>88</v>
       </c>
       <c r="G53" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="H53" t="s">
-        <v>346</v>
+        <v>36</v>
       </c>
       <c r="I53" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="J53" t="s">
-        <v>212</v>
+        <v>152</v>
       </c>
       <c r="K53" t="s">
-        <v>390</v>
+        <v>121</v>
       </c>
       <c r="L53" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="M53" t="s">
+        <v>129</v>
+      </c>
+      <c r="N53" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>336</v>
+        <v>720</v>
       </c>
       <c r="B54" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C54" t="s">
         <v>8</v>
       </c>
       <c r="D54" t="s">
-        <v>83</v>
+        <v>225</v>
       </c>
       <c r="E54" t="s">
-        <v>120</v>
+        <v>258</v>
       </c>
       <c r="F54" t="s">
-        <v>106</v>
+        <v>244</v>
       </c>
       <c r="G54" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="H54" t="s">
-        <v>113</v>
+        <v>44</v>
       </c>
       <c r="I54" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="J54" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="K54" t="s">
-        <v>276</v>
+        <v>352</v>
       </c>
       <c r="L54" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+      <c r="M54" t="s">
+        <v>327</v>
+      </c>
+      <c r="N54" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>720</v>
+        <v>24</v>
       </c>
       <c r="B55" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C55" t="s">
         <v>8</v>
       </c>
       <c r="D55" t="s">
-        <v>80</v>
+        <v>184</v>
       </c>
       <c r="E55" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="F55" t="s">
-        <v>81</v>
+        <v>147</v>
       </c>
       <c r="G55" t="s">
-        <v>267</v>
+        <v>99</v>
       </c>
       <c r="H55" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="I55" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="J55" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="K55" t="s">
-        <v>295</v>
+        <v>169</v>
       </c>
       <c r="L55" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+      <c r="M55" t="s">
+        <v>146</v>
+      </c>
+      <c r="N55" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="B56" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C56" t="s">
         <v>8</v>
       </c>
       <c r="D56" t="s">
-        <v>31</v>
+        <v>81</v>
       </c>
       <c r="E56" t="s">
-        <v>182</v>
+        <v>136</v>
       </c>
       <c r="F56" t="s">
-        <v>247</v>
+        <v>112</v>
       </c>
       <c r="G56" t="s">
-        <v>182</v>
+        <v>265</v>
       </c>
       <c r="H56" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="I56" t="s">
-        <v>27</v>
+        <v>83</v>
       </c>
       <c r="J56" t="s">
-        <v>108</v>
+        <v>181</v>
       </c>
       <c r="K56" t="s">
-        <v>391</v>
+        <v>20</v>
       </c>
       <c r="L56" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+        <v>402</v>
+      </c>
+      <c r="M56" t="s">
+        <v>341</v>
+      </c>
+      <c r="N56" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>96</v>
+        <v>192</v>
       </c>
       <c r="B57" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C57" t="s">
         <v>8</v>
       </c>
       <c r="D57" t="s">
-        <v>186</v>
+        <v>286</v>
       </c>
       <c r="E57" t="s">
-        <v>126</v>
+        <v>196</v>
       </c>
       <c r="F57" t="s">
-        <v>28</v>
+        <v>245</v>
       </c>
       <c r="G57" t="s">
-        <v>33</v>
+        <v>266</v>
       </c>
       <c r="H57" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="I57" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="J57" t="s">
-        <v>213</v>
+        <v>152</v>
       </c>
       <c r="K57" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="L57" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+      <c r="M57" t="s">
+        <v>554</v>
+      </c>
+      <c r="N57" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>192</v>
+        <v>336</v>
       </c>
       <c r="B58" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C58" t="s">
         <v>8</v>
       </c>
       <c r="D58" t="s">
-        <v>188</v>
+        <v>287</v>
       </c>
       <c r="E58" t="s">
-        <v>224</v>
+        <v>46</v>
       </c>
       <c r="F58" t="s">
-        <v>112</v>
+        <v>225</v>
       </c>
       <c r="G58" t="s">
-        <v>222</v>
+        <v>84</v>
       </c>
       <c r="H58" t="s">
-        <v>329</v>
+        <v>271</v>
       </c>
       <c r="I58" t="s">
-        <v>86</v>
+        <v>42</v>
       </c>
       <c r="J58" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="K58" t="s">
-        <v>368</v>
+        <v>387</v>
       </c>
       <c r="L58" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+      <c r="M58" t="s">
+        <v>166</v>
+      </c>
+      <c r="N58" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>336</v>
+        <v>720</v>
       </c>
       <c r="B59" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C59" t="s">
         <v>8</v>
       </c>
       <c r="D59" t="s">
-        <v>289</v>
+        <v>94</v>
       </c>
       <c r="E59" t="s">
-        <v>306</v>
+        <v>81</v>
       </c>
       <c r="F59" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G59" t="s">
-        <v>268</v>
+        <v>225</v>
       </c>
       <c r="H59" t="s">
-        <v>163</v>
+        <v>249</v>
       </c>
       <c r="I59" t="s">
-        <v>91</v>
+        <v>38</v>
       </c>
       <c r="J59" t="s">
-        <v>125</v>
+        <v>209</v>
       </c>
       <c r="K59" t="s">
-        <v>384</v>
+        <v>205</v>
       </c>
       <c r="L59" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+        <v>403</v>
+      </c>
+      <c r="M59" t="s">
+        <v>36</v>
+      </c>
+      <c r="N59" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>720</v>
+        <v>24</v>
       </c>
       <c r="B60" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C60" t="s">
         <v>8</v>
       </c>
       <c r="D60" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E60" t="s">
-        <v>307</v>
+        <v>32</v>
       </c>
       <c r="F60" t="s">
-        <v>249</v>
+        <v>68</v>
       </c>
       <c r="G60" t="s">
-        <v>269</v>
+        <v>16</v>
       </c>
       <c r="H60" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="I60" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="J60" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="K60" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="L60" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+      <c r="M60" t="s">
+        <v>555</v>
+      </c>
+      <c r="N60" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="B61" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C61" t="s">
         <v>8</v>
       </c>
       <c r="D61" t="s">
-        <v>103</v>
+        <v>201</v>
       </c>
       <c r="E61" t="s">
-        <v>102</v>
+        <v>305</v>
       </c>
       <c r="F61" t="s">
-        <v>213</v>
+        <v>179</v>
       </c>
       <c r="G61" t="s">
-        <v>168</v>
+        <v>211</v>
       </c>
       <c r="H61" t="s">
-        <v>351</v>
+        <v>12</v>
       </c>
       <c r="I61" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="J61" t="s">
-        <v>90</v>
+        <v>211</v>
       </c>
       <c r="K61" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="L61" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+        <v>404</v>
+      </c>
+      <c r="M61" t="s">
+        <v>556</v>
+      </c>
+      <c r="N61" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>96</v>
+        <v>192</v>
       </c>
       <c r="B62" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C62" t="s">
         <v>8</v>
       </c>
       <c r="D62" t="s">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c r="E62" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F62" t="s">
-        <v>158</v>
+        <v>194</v>
       </c>
       <c r="G62" t="s">
-        <v>243</v>
+        <v>134</v>
       </c>
       <c r="H62" t="s">
-        <v>109</v>
+        <v>346</v>
       </c>
       <c r="I62" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="J62" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="K62" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="L62" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+      <c r="M62" t="s">
+        <v>490</v>
+      </c>
+      <c r="N62" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>192</v>
+        <v>336</v>
       </c>
       <c r="B63" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C63" t="s">
         <v>8</v>
       </c>
       <c r="D63" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
       <c r="E63" t="s">
-        <v>17</v>
+        <v>120</v>
       </c>
       <c r="F63" t="s">
-        <v>18</v>
+        <v>106</v>
       </c>
       <c r="G63" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="H63" t="s">
-        <v>148</v>
+        <v>113</v>
       </c>
       <c r="I63" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="J63" t="s">
-        <v>180</v>
+        <v>100</v>
       </c>
       <c r="K63" t="s">
-        <v>375</v>
+        <v>276</v>
       </c>
       <c r="L63" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="M63" t="s">
+        <v>175</v>
+      </c>
+      <c r="N63" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>336</v>
+        <v>720</v>
       </c>
       <c r="B64" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C64" t="s">
         <v>8</v>
       </c>
       <c r="D64" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="E64" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F64" t="s">
-        <v>250</v>
+        <v>81</v>
       </c>
       <c r="G64" t="s">
-        <v>170</v>
+        <v>267</v>
       </c>
       <c r="H64" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="I64" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="J64" t="s">
-        <v>151</v>
+        <v>46</v>
       </c>
       <c r="K64" t="s">
-        <v>116</v>
+        <v>295</v>
       </c>
       <c r="L64" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="M64" t="s">
+        <v>125</v>
+      </c>
+      <c r="N64" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>720</v>
+        <v>24</v>
       </c>
       <c r="B65" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C65" t="s">
         <v>8</v>
       </c>
       <c r="D65" t="s">
-        <v>256</v>
+        <v>31</v>
       </c>
       <c r="E65" t="s">
-        <v>142</v>
+        <v>182</v>
       </c>
       <c r="F65" t="s">
-        <v>88</v>
+        <v>247</v>
       </c>
       <c r="G65" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="H65" t="s">
-        <v>328</v>
+        <v>348</v>
       </c>
       <c r="I65" t="s">
-        <v>71</v>
+        <v>27</v>
       </c>
       <c r="J65" t="s">
-        <v>156</v>
+        <v>108</v>
       </c>
       <c r="K65" t="s">
-        <v>51</v>
+        <v>391</v>
       </c>
       <c r="L65" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+        <v>405</v>
+      </c>
+      <c r="M65" t="s">
+        <v>391</v>
+      </c>
+      <c r="N65" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="B66" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C66" t="s">
         <v>8</v>
       </c>
       <c r="D66" t="s">
-        <v>291</v>
+        <v>186</v>
       </c>
       <c r="E66" t="s">
-        <v>308</v>
+        <v>126</v>
       </c>
       <c r="F66" t="s">
-        <v>172</v>
+        <v>28</v>
       </c>
       <c r="G66" t="s">
-        <v>270</v>
+        <v>33</v>
       </c>
       <c r="H66" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="I66" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="J66" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="K66" t="s">
-        <v>362</v>
+        <v>392</v>
       </c>
       <c r="L66" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+        <v>406</v>
+      </c>
+      <c r="M66" t="s">
+        <v>434</v>
+      </c>
+      <c r="N66" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>36</v>
+        <v>192</v>
       </c>
       <c r="B67" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C67" t="s">
         <v>8</v>
       </c>
       <c r="D67" t="s">
-        <v>292</v>
+        <v>188</v>
       </c>
       <c r="E67" t="s">
-        <v>309</v>
+        <v>224</v>
       </c>
       <c r="F67" t="s">
-        <v>251</v>
+        <v>112</v>
       </c>
       <c r="G67" t="s">
-        <v>271</v>
+        <v>222</v>
       </c>
       <c r="H67" t="s">
-        <v>354</v>
+        <v>329</v>
       </c>
       <c r="I67" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="J67" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
       <c r="K67" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
       <c r="L67" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+        <v>371</v>
+      </c>
+      <c r="M67" t="s">
+        <v>279</v>
+      </c>
+      <c r="N67" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>48</v>
+        <v>336</v>
       </c>
       <c r="B68" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C68" t="s">
         <v>8</v>
       </c>
       <c r="D68" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="E68" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F68" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="G68" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="H68" t="s">
-        <v>355</v>
+        <v>163</v>
       </c>
       <c r="I68" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="J68" t="s">
-        <v>218</v>
+        <v>125</v>
       </c>
       <c r="K68" t="s">
-        <v>364</v>
+        <v>384</v>
       </c>
       <c r="L68" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+      <c r="M68" t="s">
+        <v>129</v>
+      </c>
+      <c r="N68" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>60</v>
+        <v>720</v>
       </c>
       <c r="B69" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C69" t="s">
         <v>8</v>
       </c>
       <c r="D69" t="s">
+        <v>290</v>
+      </c>
+      <c r="E69" t="s">
+        <v>307</v>
+      </c>
+      <c r="F69" t="s">
+        <v>249</v>
+      </c>
+      <c r="G69" t="s">
+        <v>269</v>
+      </c>
+      <c r="H69" t="s">
+        <v>350</v>
+      </c>
+      <c r="I69" t="s">
+        <v>92</v>
+      </c>
+      <c r="J69" t="s">
+        <v>214</v>
+      </c>
+      <c r="K69" t="s">
+        <v>393</v>
+      </c>
+      <c r="L69" t="s">
+        <v>407</v>
+      </c>
+      <c r="M69" t="s">
+        <v>435</v>
+      </c>
+      <c r="N69" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>24</v>
+      </c>
+      <c r="B70" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70" t="s">
+        <v>8</v>
+      </c>
+      <c r="D70" t="s">
+        <v>103</v>
+      </c>
+      <c r="E70" t="s">
+        <v>102</v>
+      </c>
+      <c r="F70" t="s">
+        <v>213</v>
+      </c>
+      <c r="G70" t="s">
+        <v>168</v>
+      </c>
+      <c r="H70" t="s">
+        <v>351</v>
+      </c>
+      <c r="I70" t="s">
+        <v>68</v>
+      </c>
+      <c r="J70" t="s">
+        <v>90</v>
+      </c>
+      <c r="K70" t="s">
+        <v>394</v>
+      </c>
+      <c r="L70" t="s">
+        <v>408</v>
+      </c>
+      <c r="M70" t="s">
+        <v>90</v>
+      </c>
+      <c r="N70" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>96</v>
+      </c>
+      <c r="B71" t="s">
+        <v>5</v>
+      </c>
+      <c r="C71" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71" t="s">
+        <v>140</v>
+      </c>
+      <c r="E71" t="s">
+        <v>140</v>
+      </c>
+      <c r="F71" t="s">
+        <v>158</v>
+      </c>
+      <c r="G71" t="s">
+        <v>243</v>
+      </c>
+      <c r="H71" t="s">
+        <v>109</v>
+      </c>
+      <c r="I71" t="s">
+        <v>69</v>
+      </c>
+      <c r="J71" t="s">
+        <v>215</v>
+      </c>
+      <c r="K71" t="s">
+        <v>395</v>
+      </c>
+      <c r="L71" t="s">
+        <v>409</v>
+      </c>
+      <c r="M71" t="s">
+        <v>158</v>
+      </c>
+      <c r="N71" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>192</v>
+      </c>
+      <c r="B72" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" t="s">
+        <v>17</v>
+      </c>
+      <c r="E72" t="s">
+        <v>17</v>
+      </c>
+      <c r="F72" t="s">
+        <v>18</v>
+      </c>
+      <c r="G72" t="s">
+        <v>169</v>
+      </c>
+      <c r="H72" t="s">
+        <v>148</v>
+      </c>
+      <c r="I72" t="s">
+        <v>12</v>
+      </c>
+      <c r="J72" t="s">
+        <v>180</v>
+      </c>
+      <c r="K72" t="s">
+        <v>375</v>
+      </c>
+      <c r="L72" t="s">
+        <v>147</v>
+      </c>
+      <c r="M72" t="s">
+        <v>180</v>
+      </c>
+      <c r="N72" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>336</v>
+      </c>
+      <c r="B73" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" t="s">
+        <v>29</v>
+      </c>
+      <c r="E73" t="s">
+        <v>141</v>
+      </c>
+      <c r="F73" t="s">
+        <v>250</v>
+      </c>
+      <c r="G73" t="s">
+        <v>170</v>
+      </c>
+      <c r="H73" t="s">
+        <v>352</v>
+      </c>
+      <c r="I73" t="s">
+        <v>70</v>
+      </c>
+      <c r="J73" t="s">
+        <v>151</v>
+      </c>
+      <c r="K73" t="s">
+        <v>116</v>
+      </c>
+      <c r="L73" t="s">
+        <v>369</v>
+      </c>
+      <c r="M73" t="s">
+        <v>482</v>
+      </c>
+      <c r="N73" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>720</v>
+      </c>
+      <c r="B74" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" t="s">
+        <v>256</v>
+      </c>
+      <c r="E74" t="s">
+        <v>142</v>
+      </c>
+      <c r="F74" t="s">
+        <v>88</v>
+      </c>
+      <c r="G74" t="s">
+        <v>171</v>
+      </c>
+      <c r="H74" t="s">
+        <v>328</v>
+      </c>
+      <c r="I74" t="s">
+        <v>71</v>
+      </c>
+      <c r="J74" t="s">
+        <v>156</v>
+      </c>
+      <c r="K74" t="s">
+        <v>51</v>
+      </c>
+      <c r="L74" t="s">
+        <v>156</v>
+      </c>
+      <c r="M74" t="s">
+        <v>21</v>
+      </c>
+      <c r="N74" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>24</v>
+      </c>
+      <c r="B75" t="s">
+        <v>6</v>
+      </c>
+      <c r="C75" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75" t="s">
+        <v>291</v>
+      </c>
+      <c r="E75" t="s">
+        <v>308</v>
+      </c>
+      <c r="F75" t="s">
+        <v>172</v>
+      </c>
+      <c r="G75" t="s">
+        <v>270</v>
+      </c>
+      <c r="H75" t="s">
+        <v>353</v>
+      </c>
+      <c r="I75" t="s">
+        <v>67</v>
+      </c>
+      <c r="J75" t="s">
+        <v>216</v>
+      </c>
+      <c r="K75" t="s">
+        <v>362</v>
+      </c>
+      <c r="L75" t="s">
+        <v>414</v>
+      </c>
+      <c r="M75" t="s">
+        <v>436</v>
+      </c>
+      <c r="N75" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>36</v>
+      </c>
+      <c r="B76" t="s">
+        <v>6</v>
+      </c>
+      <c r="C76" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76" t="s">
+        <v>292</v>
+      </c>
+      <c r="E76" t="s">
+        <v>309</v>
+      </c>
+      <c r="F76" t="s">
+        <v>251</v>
+      </c>
+      <c r="G76" t="s">
+        <v>271</v>
+      </c>
+      <c r="H76" t="s">
+        <v>354</v>
+      </c>
+      <c r="I76" t="s">
+        <v>65</v>
+      </c>
+      <c r="J76" t="s">
+        <v>217</v>
+      </c>
+      <c r="K76" t="s">
+        <v>363</v>
+      </c>
+      <c r="L76" t="s">
+        <v>415</v>
+      </c>
+      <c r="M76" t="s">
+        <v>437</v>
+      </c>
+      <c r="N76" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>48</v>
+      </c>
+      <c r="B77" t="s">
+        <v>6</v>
+      </c>
+      <c r="C77" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" t="s">
+        <v>293</v>
+      </c>
+      <c r="E77" t="s">
+        <v>310</v>
+      </c>
+      <c r="F77" t="s">
+        <v>252</v>
+      </c>
+      <c r="G77" t="s">
+        <v>272</v>
+      </c>
+      <c r="H77" t="s">
+        <v>355</v>
+      </c>
+      <c r="I77" t="s">
+        <v>65</v>
+      </c>
+      <c r="J77" t="s">
+        <v>218</v>
+      </c>
+      <c r="K77" t="s">
+        <v>364</v>
+      </c>
+      <c r="L77" t="s">
+        <v>416</v>
+      </c>
+      <c r="M77" t="s">
+        <v>438</v>
+      </c>
+      <c r="N77" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>60</v>
+      </c>
+      <c r="B78" t="s">
+        <v>6</v>
+      </c>
+      <c r="C78" t="s">
+        <v>8</v>
+      </c>
+      <c r="D78" t="s">
         <v>294</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E78" t="s">
         <v>311</v>
       </c>
-      <c r="F69" t="s">
+      <c r="F78" t="s">
         <v>253</v>
       </c>
-      <c r="G69" t="s">
+      <c r="G78" t="s">
         <v>273</v>
       </c>
-      <c r="H69" t="s">
+      <c r="H78" t="s">
         <v>356</v>
       </c>
-      <c r="I69" t="s">
+      <c r="I78" t="s">
         <v>66</v>
       </c>
-      <c r="J69" t="s">
+      <c r="J78" t="s">
         <v>219</v>
       </c>
-      <c r="K69" t="s">
+      <c r="K78" t="s">
         <v>365</v>
       </c>
-      <c r="L69" t="s">
+      <c r="L78" t="s">
         <v>417</v>
+      </c>
+      <c r="M78" t="s">
+        <v>439</v>
+      </c>
+      <c r="N78" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>24</v>
+      </c>
+      <c r="B79" t="s">
+        <v>483</v>
+      </c>
+      <c r="C79" t="s">
+        <v>8</v>
+      </c>
+      <c r="D79" t="s">
+        <v>558</v>
+      </c>
+      <c r="E79" t="s">
+        <v>86</v>
+      </c>
+      <c r="F79" t="s">
+        <v>82</v>
+      </c>
+      <c r="G79" t="s">
+        <v>525</v>
+      </c>
+      <c r="H79" t="s">
+        <v>518</v>
+      </c>
+      <c r="I79" t="s">
+        <v>295</v>
+      </c>
+      <c r="J79" t="s">
+        <v>534</v>
+      </c>
+      <c r="K79" t="s">
+        <v>41</v>
+      </c>
+      <c r="L79" t="s">
+        <v>274</v>
+      </c>
+      <c r="M79" t="s">
+        <v>30</v>
+      </c>
+      <c r="N79" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>36</v>
+      </c>
+      <c r="B80" t="s">
+        <v>483</v>
+      </c>
+      <c r="C80" t="s">
+        <v>8</v>
+      </c>
+      <c r="D80" t="s">
+        <v>57</v>
+      </c>
+      <c r="E80" t="s">
+        <v>104</v>
+      </c>
+      <c r="F80" t="s">
+        <v>20</v>
+      </c>
+      <c r="G80" t="s">
+        <v>75</v>
+      </c>
+      <c r="H80" t="s">
+        <v>519</v>
+      </c>
+      <c r="I80" t="s">
+        <v>254</v>
+      </c>
+      <c r="J80" t="s">
+        <v>535</v>
+      </c>
+      <c r="K80" t="s">
+        <v>491</v>
+      </c>
+      <c r="L80" t="s">
+        <v>242</v>
+      </c>
+      <c r="M80" t="s">
+        <v>486</v>
+      </c>
+      <c r="N80" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>48</v>
+      </c>
+      <c r="B81" t="s">
+        <v>483</v>
+      </c>
+      <c r="C81" t="s">
+        <v>8</v>
+      </c>
+      <c r="D81" t="s">
+        <v>398</v>
+      </c>
+      <c r="E81" t="s">
+        <v>29</v>
+      </c>
+      <c r="F81" t="s">
+        <v>52</v>
+      </c>
+      <c r="G81" t="s">
+        <v>496</v>
+      </c>
+      <c r="H81" t="s">
+        <v>437</v>
+      </c>
+      <c r="I81" t="s">
+        <v>530</v>
+      </c>
+      <c r="J81" t="s">
+        <v>392</v>
+      </c>
+      <c r="K81" t="s">
+        <v>492</v>
+      </c>
+      <c r="L81" t="s">
+        <v>500</v>
+      </c>
+      <c r="M81" t="s">
+        <v>146</v>
+      </c>
+      <c r="N81" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>60</v>
+      </c>
+      <c r="B82" t="s">
+        <v>483</v>
+      </c>
+      <c r="C82" t="s">
+        <v>8</v>
+      </c>
+      <c r="D82" t="s">
+        <v>184</v>
+      </c>
+      <c r="E82" t="s">
+        <v>390</v>
+      </c>
+      <c r="F82" t="s">
+        <v>188</v>
+      </c>
+      <c r="G82" t="s">
+        <v>189</v>
+      </c>
+      <c r="H82" t="s">
+        <v>333</v>
+      </c>
+      <c r="I82" t="s">
+        <v>531</v>
+      </c>
+      <c r="J82" t="s">
+        <v>32</v>
+      </c>
+      <c r="K82" t="s">
+        <v>493</v>
+      </c>
+      <c r="L82" t="s">
+        <v>501</v>
+      </c>
+      <c r="M82" t="s">
+        <v>56</v>
+      </c>
+      <c r="N82" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>24</v>
+      </c>
+      <c r="B83" t="s">
+        <v>484</v>
+      </c>
+      <c r="C83" t="s">
+        <v>8</v>
+      </c>
+      <c r="D83" t="s">
+        <v>534</v>
+      </c>
+      <c r="E83" t="s">
+        <v>569</v>
+      </c>
+      <c r="F83" t="s">
+        <v>494</v>
+      </c>
+      <c r="G83" t="s">
+        <v>565</v>
+      </c>
+      <c r="H83" t="s">
+        <v>520</v>
+      </c>
+      <c r="I83" t="s">
+        <v>532</v>
+      </c>
+      <c r="J83" t="s">
+        <v>378</v>
+      </c>
+      <c r="K83" t="s">
+        <v>494</v>
+      </c>
+      <c r="L83" t="s">
+        <v>502</v>
+      </c>
+      <c r="M83" t="s">
+        <v>388</v>
+      </c>
+      <c r="N83" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>96</v>
+      </c>
+      <c r="B84" t="s">
+        <v>484</v>
+      </c>
+      <c r="C84" t="s">
+        <v>8</v>
+      </c>
+      <c r="D84" t="s">
+        <v>559</v>
+      </c>
+      <c r="E84" t="s">
+        <v>388</v>
+      </c>
+      <c r="F84" t="s">
+        <v>503</v>
+      </c>
+      <c r="G84" t="s">
+        <v>380</v>
+      </c>
+      <c r="H84" t="s">
+        <v>521</v>
+      </c>
+      <c r="I84" t="s">
+        <v>533</v>
+      </c>
+      <c r="J84" t="s">
+        <v>486</v>
+      </c>
+      <c r="K84" t="s">
+        <v>406</v>
+      </c>
+      <c r="L84" t="s">
+        <v>503</v>
+      </c>
+      <c r="M84" t="s">
+        <v>487</v>
+      </c>
+      <c r="N84" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>192</v>
+      </c>
+      <c r="B85" t="s">
+        <v>484</v>
+      </c>
+      <c r="C85" t="s">
+        <v>8</v>
+      </c>
+      <c r="D85" t="s">
+        <v>211</v>
+      </c>
+      <c r="E85" t="s">
+        <v>140</v>
+      </c>
+      <c r="F85" t="s">
+        <v>389</v>
+      </c>
+      <c r="G85" t="s">
+        <v>33</v>
+      </c>
+      <c r="H85" t="s">
+        <v>522</v>
+      </c>
+      <c r="I85" t="s">
+        <v>169</v>
+      </c>
+      <c r="J85" t="s">
+        <v>508</v>
+      </c>
+      <c r="K85" t="s">
+        <v>385</v>
+      </c>
+      <c r="L85" t="s">
+        <v>305</v>
+      </c>
+      <c r="M85" t="s">
+        <v>77</v>
+      </c>
+      <c r="N85" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>336</v>
+      </c>
+      <c r="B86" t="s">
+        <v>484</v>
+      </c>
+      <c r="C86" t="s">
+        <v>8</v>
+      </c>
+      <c r="D86" t="s">
+        <v>57</v>
+      </c>
+      <c r="E86" t="s">
+        <v>279</v>
+      </c>
+      <c r="F86" t="s">
+        <v>18</v>
+      </c>
+      <c r="G86" t="s">
+        <v>566</v>
+      </c>
+      <c r="H86" t="s">
+        <v>523</v>
+      </c>
+      <c r="I86" t="s">
+        <v>229</v>
+      </c>
+      <c r="J86" t="s">
+        <v>390</v>
+      </c>
+      <c r="K86" t="s">
+        <v>212</v>
+      </c>
+      <c r="L86" t="s">
+        <v>504</v>
+      </c>
+      <c r="M86" t="s">
+        <v>138</v>
+      </c>
+      <c r="N86" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>720</v>
+      </c>
+      <c r="B87" t="s">
+        <v>484</v>
+      </c>
+      <c r="C87" t="s">
+        <v>8</v>
+      </c>
+      <c r="D87" t="s">
+        <v>232</v>
+      </c>
+      <c r="E87" t="s">
+        <v>481</v>
+      </c>
+      <c r="F87" t="s">
+        <v>507</v>
+      </c>
+      <c r="G87" t="s">
+        <v>173</v>
+      </c>
+      <c r="H87" t="s">
+        <v>524</v>
+      </c>
+      <c r="I87" t="s">
+        <v>45</v>
+      </c>
+      <c r="J87" t="s">
+        <v>70</v>
+      </c>
+      <c r="K87" t="s">
+        <v>495</v>
+      </c>
+      <c r="L87" t="s">
+        <v>505</v>
+      </c>
+      <c r="M87" t="s">
+        <v>162</v>
+      </c>
+      <c r="N87" t="s">
+        <v>552</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new notebooks and update ex
</commit_message>
<xml_diff>
--- a/Experiment_results/xlsx_format/ex_multi.xlsx
+++ b/Experiment_results/xlsx_format/ex_multi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\ДИПЛОМНЫЙ проект\результаты экспериментов\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B923ACB-41BE-4A88-9707-3495A1EB6DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65BFF9B0-E38E-4639-9715-8B589570BFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист2" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1306" uniqueCount="639">
   <si>
     <t>ETTh1</t>
   </si>
@@ -1747,6 +1747,210 @@
   </si>
   <si>
     <t>Repeat_Closest</t>
+  </si>
+  <si>
+    <t>UniTime_8 (zero-shot)</t>
+  </si>
+  <si>
+    <t>UniTime_8 (finetune)</t>
+  </si>
+  <si>
+    <t>0.613</t>
+  </si>
+  <si>
+    <t>0.636</t>
+  </si>
+  <si>
+    <t>0.652</t>
+  </si>
+  <si>
+    <t>0.357</t>
+  </si>
+  <si>
+    <t>0.478</t>
+  </si>
+  <si>
+    <t>0.610</t>
+  </si>
+  <si>
+    <t>0.617</t>
+  </si>
+  <si>
+    <t>0.361</t>
+  </si>
+  <si>
+    <t>0.460</t>
+  </si>
+  <si>
+    <t>0.738</t>
+  </si>
+  <si>
+    <t>1.583</t>
+  </si>
+  <si>
+    <t>0.393</t>
+  </si>
+  <si>
+    <t>1.291</t>
+  </si>
+  <si>
+    <t>1.193</t>
+  </si>
+  <si>
+    <t>1.105</t>
+  </si>
+  <si>
+    <t>1.094</t>
+  </si>
+  <si>
+    <t>1.119</t>
+  </si>
+  <si>
+    <t>0.963</t>
+  </si>
+  <si>
+    <t>0.983</t>
+  </si>
+  <si>
+    <t>1.020</t>
+  </si>
+  <si>
+    <t>0.847</t>
+  </si>
+  <si>
+    <t>0.880</t>
+  </si>
+  <si>
+    <t>0.883</t>
+  </si>
+  <si>
+    <t>0.286</t>
+  </si>
+  <si>
+    <t>0.472</t>
+  </si>
+  <si>
+    <t>0.498</t>
+  </si>
+  <si>
+    <t>0.497</t>
+  </si>
+  <si>
+    <t>1.030</t>
+  </si>
+  <si>
+    <t>0.872</t>
+  </si>
+  <si>
+    <t>0.882</t>
+  </si>
+  <si>
+    <t>0.918</t>
+  </si>
+  <si>
+    <t>0.210</t>
+  </si>
+  <si>
+    <t>0.467</t>
+  </si>
+  <si>
+    <t>0.938</t>
+  </si>
+  <si>
+    <t>5.737</t>
+  </si>
+  <si>
+    <t>3.829</t>
+  </si>
+  <si>
+    <t>3.267</t>
+  </si>
+  <si>
+    <t>3.073</t>
+  </si>
+  <si>
+    <t>1.864</t>
+  </si>
+  <si>
+    <t>1.771</t>
+  </si>
+  <si>
+    <t>1.835</t>
+  </si>
+  <si>
+    <t>1.534</t>
+  </si>
+  <si>
+    <t>1.371</t>
+  </si>
+  <si>
+    <t>1.550</t>
+  </si>
+  <si>
+    <t>0.482</t>
+  </si>
+  <si>
+    <t>0.456</t>
+  </si>
+  <si>
+    <t>0.408</t>
+  </si>
+  <si>
+    <t>0.217</t>
+  </si>
+  <si>
+    <t>0.209</t>
+  </si>
+  <si>
+    <t>0.705</t>
+  </si>
+  <si>
+    <t>0.347</t>
+  </si>
+  <si>
+    <t>1.040</t>
+  </si>
+  <si>
+    <t>0.980</t>
+  </si>
+  <si>
+    <t>0.971</t>
+  </si>
+  <si>
+    <t>0.978</t>
+  </si>
+  <si>
+    <t>0.445</t>
+  </si>
+  <si>
+    <t>0.469</t>
+  </si>
+  <si>
+    <t>0.464</t>
+  </si>
+  <si>
+    <t>0.479</t>
+  </si>
+  <si>
+    <t>0.434</t>
+  </si>
+  <si>
+    <t>0.029</t>
+  </si>
+  <si>
+    <t>3.006</t>
+  </si>
+  <si>
+    <t>2.463</t>
+  </si>
+  <si>
+    <t>2.360</t>
+  </si>
+  <si>
+    <t>2.230</t>
+  </si>
+  <si>
+    <t>0.316</t>
   </si>
 </sst>
 </file>
@@ -2065,10 +2269,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6080771B-968D-4139-AF07-E0D46FA87262}">
-  <dimension ref="A1:N87"/>
+  <dimension ref="A1:P87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection activeCell="I83" sqref="I83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2079,16 +2283,18 @@
     <col min="5" max="5" width="19.88671875" customWidth="1"/>
     <col min="6" max="6" width="18.44140625" customWidth="1"/>
     <col min="7" max="7" width="17.77734375" customWidth="1"/>
-    <col min="8" max="8" width="18.88671875" customWidth="1"/>
-    <col min="9" max="9" width="18.109375" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" customWidth="1"/>
-    <col min="11" max="11" width="9.109375" customWidth="1"/>
-    <col min="12" max="12" width="9.44140625" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" customWidth="1"/>
-    <col min="14" max="14" width="11.109375" customWidth="1"/>
+    <col min="8" max="8" width="19.21875" customWidth="1"/>
+    <col min="9" max="9" width="17.77734375" customWidth="1"/>
+    <col min="10" max="10" width="18.88671875" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" customWidth="1"/>
+    <col min="12" max="12" width="9.6640625" customWidth="1"/>
+    <col min="13" max="13" width="9.109375" customWidth="1"/>
+    <col min="14" max="14" width="9.44140625" customWidth="1"/>
+    <col min="15" max="15" width="10.44140625" customWidth="1"/>
+    <col min="16" max="16" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>96</v>
       </c>
@@ -2111,28 +2317,34 @@
         <v>422</v>
       </c>
       <c r="H1" t="s">
+        <v>571</v>
+      </c>
+      <c r="I1" t="s">
+        <v>572</v>
+      </c>
+      <c r="J1" t="s">
         <v>312</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>418</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>366</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>357</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>423</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>424</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>24</v>
       </c>
@@ -2155,28 +2367,34 @@
         <v>148</v>
       </c>
       <c r="H2" t="s">
+        <v>473</v>
+      </c>
+      <c r="I2" t="s">
+        <v>166</v>
+      </c>
+      <c r="J2" t="s">
         <v>313</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>26</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>157</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>121</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>208</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>125</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>96</v>
       </c>
@@ -2199,28 +2417,34 @@
         <v>135</v>
       </c>
       <c r="H3" t="s">
+        <v>573</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
         <v>314</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>36</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>188</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>149</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>197</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>245</v>
       </c>
-      <c r="N3" t="s">
+      <c r="P3" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>192</v>
       </c>
@@ -2243,28 +2467,34 @@
         <v>223</v>
       </c>
       <c r="H4" t="s">
+        <v>337</v>
+      </c>
+      <c r="I4" t="s">
+        <v>525</v>
+      </c>
+      <c r="J4" t="s">
         <v>315</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>37</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>189</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>42</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>397</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>26</v>
       </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>336</v>
       </c>
@@ -2287,28 +2517,34 @@
         <v>81</v>
       </c>
       <c r="H5" t="s">
+        <v>574</v>
+      </c>
+      <c r="I5" t="s">
+        <v>581</v>
+      </c>
+      <c r="J5" t="s">
         <v>316</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>38</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>190</v>
-      </c>
-      <c r="K5" t="s">
-        <v>370</v>
-      </c>
-      <c r="L5" t="s">
-        <v>164</v>
       </c>
       <c r="M5" t="s">
         <v>370</v>
       </c>
       <c r="N5" t="s">
+        <v>164</v>
+      </c>
+      <c r="O5" t="s">
+        <v>370</v>
+      </c>
+      <c r="P5" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>720</v>
       </c>
@@ -2331,28 +2567,34 @@
         <v>254</v>
       </c>
       <c r="H6" t="s">
+        <v>575</v>
+      </c>
+      <c r="I6" t="s">
+        <v>617</v>
+      </c>
+      <c r="J6" t="s">
         <v>317</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
         <v>39</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>191</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>76</v>
       </c>
-      <c r="L6" t="s">
+      <c r="N6" t="s">
         <v>297</v>
       </c>
-      <c r="M6" t="s">
+      <c r="O6" t="s">
         <v>165</v>
       </c>
-      <c r="N6" t="s">
+      <c r="P6" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>24</v>
       </c>
@@ -2375,28 +2617,34 @@
         <v>13</v>
       </c>
       <c r="H7" t="s">
+        <v>576</v>
+      </c>
+      <c r="I7" t="s">
+        <v>377</v>
+      </c>
+      <c r="J7" t="s">
         <v>25</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>40</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>120</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
         <v>250</v>
       </c>
-      <c r="L7" t="s">
+      <c r="N7" t="s">
         <v>35</v>
       </c>
-      <c r="M7" t="s">
+      <c r="O7" t="s">
         <v>426</v>
       </c>
-      <c r="N7" t="s">
+      <c r="P7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>96</v>
       </c>
@@ -2419,28 +2667,34 @@
         <v>233</v>
       </c>
       <c r="H8" t="s">
+        <v>230</v>
+      </c>
+      <c r="I8" t="s">
+        <v>52</v>
+      </c>
+      <c r="J8" t="s">
         <v>41</v>
       </c>
-      <c r="I8" t="s">
+      <c r="K8" t="s">
         <v>41</v>
       </c>
-      <c r="J8" t="s">
+      <c r="L8" t="s">
         <v>148</v>
       </c>
-      <c r="K8" t="s">
+      <c r="M8" t="s">
         <v>156</v>
       </c>
-      <c r="L8" t="s">
+      <c r="N8" t="s">
         <v>106</v>
       </c>
-      <c r="M8" t="s">
+      <c r="O8" t="s">
         <v>121</v>
       </c>
-      <c r="N8" t="s">
+      <c r="P8" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>192</v>
       </c>
@@ -2463,28 +2717,34 @@
         <v>196</v>
       </c>
       <c r="H9" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="I9" t="s">
         <v>42</v>
       </c>
       <c r="J9" t="s">
+        <v>274</v>
+      </c>
+      <c r="K9" t="s">
+        <v>42</v>
+      </c>
+      <c r="L9" t="s">
         <v>192</v>
       </c>
-      <c r="K9" t="s">
+      <c r="M9" t="s">
         <v>255</v>
       </c>
-      <c r="L9" t="s">
+      <c r="N9" t="s">
         <v>163</v>
       </c>
-      <c r="M9" t="s">
+      <c r="O9" t="s">
         <v>258</v>
       </c>
-      <c r="N9" t="s">
+      <c r="P9" t="s">
         <v>444</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>336</v>
       </c>
@@ -2507,28 +2767,34 @@
         <v>122</v>
       </c>
       <c r="H10" t="s">
+        <v>577</v>
+      </c>
+      <c r="I10" t="s">
+        <v>74</v>
+      </c>
+      <c r="J10" t="s">
         <v>115</v>
       </c>
-      <c r="I10" t="s">
+      <c r="K10" t="s">
         <v>43</v>
       </c>
-      <c r="J10" t="s">
+      <c r="L10" t="s">
         <v>192</v>
       </c>
-      <c r="K10" t="s">
+      <c r="M10" t="s">
         <v>79</v>
       </c>
-      <c r="L10" t="s">
+      <c r="N10" t="s">
         <v>157</v>
       </c>
-      <c r="M10" t="s">
+      <c r="O10" t="s">
         <v>149</v>
       </c>
-      <c r="N10" t="s">
+      <c r="P10" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>720</v>
       </c>
@@ -2551,28 +2817,34 @@
         <v>48</v>
       </c>
       <c r="H11" t="s">
+        <v>246</v>
+      </c>
+      <c r="I11" t="s">
+        <v>618</v>
+      </c>
+      <c r="J11" t="s">
         <v>318</v>
       </c>
-      <c r="I11" t="s">
+      <c r="K11" t="s">
         <v>44</v>
       </c>
-      <c r="J11" t="s">
+      <c r="L11" t="s">
         <v>193</v>
       </c>
-      <c r="K11" t="s">
+      <c r="M11" t="s">
         <v>373</v>
       </c>
-      <c r="L11" t="s">
+      <c r="N11" t="s">
         <v>164</v>
       </c>
-      <c r="M11" t="s">
+      <c r="O11" t="s">
         <v>115</v>
       </c>
-      <c r="N11" t="s">
+      <c r="P11" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>24</v>
       </c>
@@ -2595,28 +2867,34 @@
         <v>138</v>
       </c>
       <c r="H12" t="s">
+        <v>235</v>
+      </c>
+      <c r="I12" t="s">
+        <v>171</v>
+      </c>
+      <c r="J12" t="s">
         <v>322</v>
       </c>
-      <c r="I12" t="s">
+      <c r="K12" t="s">
         <v>45</v>
       </c>
-      <c r="J12" t="s">
+      <c r="L12" t="s">
         <v>194</v>
       </c>
-      <c r="K12" t="s">
+      <c r="M12" t="s">
         <v>227</v>
       </c>
-      <c r="L12" t="s">
+      <c r="N12" t="s">
         <v>131</v>
       </c>
-      <c r="M12" t="s">
+      <c r="O12" t="s">
         <v>495</v>
       </c>
-      <c r="N12" t="s">
+      <c r="P12" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>96</v>
       </c>
@@ -2639,28 +2917,34 @@
         <v>106</v>
       </c>
       <c r="H13" t="s">
+        <v>527</v>
+      </c>
+      <c r="I13" t="s">
+        <v>84</v>
+      </c>
+      <c r="J13" t="s">
         <v>323</v>
       </c>
-      <c r="I13" t="s">
+      <c r="K13" t="s">
         <v>46</v>
       </c>
-      <c r="J13" t="s">
+      <c r="L13" t="s">
         <v>139</v>
       </c>
-      <c r="K13" t="s">
+      <c r="M13" t="s">
         <v>167</v>
       </c>
-      <c r="L13" t="s">
+      <c r="N13" t="s">
         <v>71</v>
       </c>
-      <c r="M13" t="s">
+      <c r="O13" t="s">
         <v>384</v>
       </c>
-      <c r="N13" t="s">
+      <c r="P13" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>192</v>
       </c>
@@ -2683,28 +2967,34 @@
         <v>255</v>
       </c>
       <c r="H14" t="s">
-        <v>324</v>
+        <v>578</v>
       </c>
       <c r="I14" t="s">
         <v>47</v>
       </c>
       <c r="J14" t="s">
+        <v>324</v>
+      </c>
+      <c r="K14" t="s">
+        <v>47</v>
+      </c>
+      <c r="L14" t="s">
         <v>195</v>
-      </c>
-      <c r="K14" t="s">
-        <v>125</v>
-      </c>
-      <c r="L14" t="s">
-        <v>387</v>
       </c>
       <c r="M14" t="s">
         <v>125</v>
       </c>
       <c r="N14" t="s">
+        <v>387</v>
+      </c>
+      <c r="O14" t="s">
+        <v>125</v>
+      </c>
+      <c r="P14" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>336</v>
       </c>
@@ -2727,28 +3017,34 @@
         <v>192</v>
       </c>
       <c r="H15" t="s">
+        <v>579</v>
+      </c>
+      <c r="I15" t="s">
+        <v>619</v>
+      </c>
+      <c r="J15" t="s">
         <v>325</v>
       </c>
-      <c r="I15" t="s">
+      <c r="K15" t="s">
         <v>48</v>
       </c>
-      <c r="J15" t="s">
+      <c r="L15" t="s">
         <v>11</v>
       </c>
-      <c r="K15" t="s">
+      <c r="M15" t="s">
         <v>374</v>
       </c>
-      <c r="L15" t="s">
+      <c r="N15" t="s">
         <v>22</v>
       </c>
-      <c r="M15" t="s">
+      <c r="O15" t="s">
         <v>245</v>
       </c>
-      <c r="N15" t="s">
+      <c r="P15" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>720</v>
       </c>
@@ -2771,28 +3067,34 @@
         <v>26</v>
       </c>
       <c r="H16" t="s">
+        <v>574</v>
+      </c>
+      <c r="I16" t="s">
+        <v>297</v>
+      </c>
+      <c r="J16" t="s">
         <v>326</v>
       </c>
-      <c r="I16" t="s">
+      <c r="K16" t="s">
         <v>37</v>
       </c>
-      <c r="J16" t="s">
+      <c r="L16" t="s">
         <v>36</v>
       </c>
-      <c r="K16" t="s">
+      <c r="M16" t="s">
         <v>89</v>
       </c>
-      <c r="L16" t="s">
+      <c r="N16" t="s">
         <v>80</v>
       </c>
-      <c r="M16" t="s">
+      <c r="O16" t="s">
         <v>36</v>
       </c>
-      <c r="N16" t="s">
+      <c r="P16" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>24</v>
       </c>
@@ -2815,28 +3117,34 @@
         <v>86</v>
       </c>
       <c r="H17" t="s">
+        <v>45</v>
+      </c>
+      <c r="I17" t="s">
+        <v>620</v>
+      </c>
+      <c r="J17" t="s">
         <v>13</v>
       </c>
-      <c r="I17" t="s">
+      <c r="K17" t="s">
         <v>49</v>
       </c>
-      <c r="J17" t="s">
+      <c r="L17" t="s">
         <v>143</v>
       </c>
-      <c r="K17" t="s">
+      <c r="M17" t="s">
         <v>375</v>
       </c>
-      <c r="L17" t="s">
+      <c r="N17" t="s">
         <v>396</v>
       </c>
-      <c r="M17" t="s">
+      <c r="O17" t="s">
         <v>396</v>
       </c>
-      <c r="N17" t="s">
+      <c r="P17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>96</v>
       </c>
@@ -2859,28 +3167,34 @@
         <v>257</v>
       </c>
       <c r="H18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" t="s">
         <v>233</v>
       </c>
-      <c r="I18" t="s">
+      <c r="K18" t="s">
         <v>50</v>
       </c>
-      <c r="J18" t="s">
+      <c r="L18" t="s">
         <v>174</v>
       </c>
-      <c r="K18" t="s">
+      <c r="M18" t="s">
         <v>376</v>
       </c>
-      <c r="L18" t="s">
+      <c r="N18" t="s">
         <v>398</v>
       </c>
-      <c r="M18" t="s">
+      <c r="O18" t="s">
         <v>467</v>
       </c>
-      <c r="N18" t="s">
+      <c r="P18" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>192</v>
       </c>
@@ -2903,28 +3217,34 @@
         <v>35</v>
       </c>
       <c r="H19" t="s">
+        <v>580</v>
+      </c>
+      <c r="I19" t="s">
+        <v>402</v>
+      </c>
+      <c r="J19" t="s">
         <v>267</v>
       </c>
-      <c r="I19" t="s">
+      <c r="K19" t="s">
         <v>51</v>
       </c>
-      <c r="J19" t="s">
+      <c r="L19" t="s">
         <v>181</v>
       </c>
-      <c r="K19" t="s">
+      <c r="M19" t="s">
         <v>377</v>
       </c>
-      <c r="L19" t="s">
+      <c r="N19" t="s">
         <v>265</v>
       </c>
-      <c r="M19" t="s">
+      <c r="O19" t="s">
         <v>109</v>
       </c>
-      <c r="N19" t="s">
+      <c r="P19" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>336</v>
       </c>
@@ -2947,28 +3267,34 @@
         <v>88</v>
       </c>
       <c r="H20" t="s">
+        <v>228</v>
+      </c>
+      <c r="I20" t="s">
+        <v>41</v>
+      </c>
+      <c r="J20" t="s">
         <v>327</v>
       </c>
-      <c r="I20" t="s">
+      <c r="K20" t="s">
         <v>52</v>
       </c>
-      <c r="J20" t="s">
+      <c r="L20" t="s">
         <v>196</v>
       </c>
-      <c r="K20" t="s">
+      <c r="M20" t="s">
         <v>266</v>
       </c>
-      <c r="L20" t="s">
+      <c r="N20" t="s">
         <v>372</v>
       </c>
-      <c r="M20" t="s">
+      <c r="O20" t="s">
         <v>196</v>
       </c>
-      <c r="N20" t="s">
+      <c r="P20" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>720</v>
       </c>
@@ -2991,28 +3317,34 @@
         <v>258</v>
       </c>
       <c r="H21" t="s">
+        <v>297</v>
+      </c>
+      <c r="I21" t="s">
+        <v>114</v>
+      </c>
+      <c r="J21" t="s">
         <v>328</v>
       </c>
-      <c r="I21" t="s">
+      <c r="K21" t="s">
         <v>26</v>
       </c>
-      <c r="J21" t="s">
+      <c r="L21" t="s">
         <v>197</v>
       </c>
-      <c r="K21" t="s">
+      <c r="M21" t="s">
         <v>79</v>
       </c>
-      <c r="L21" t="s">
+      <c r="N21" t="s">
         <v>101</v>
       </c>
-      <c r="M21" t="s">
+      <c r="O21" t="s">
         <v>553</v>
       </c>
-      <c r="N21" t="s">
+      <c r="P21" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>24</v>
       </c>
@@ -3035,28 +3367,34 @@
         <v>30</v>
       </c>
       <c r="H22" t="s">
+        <v>329</v>
+      </c>
+      <c r="I22" t="s">
+        <v>178</v>
+      </c>
+      <c r="J22" t="s">
         <v>56</v>
       </c>
-      <c r="I22" t="s">
+      <c r="K22" t="s">
         <v>53</v>
       </c>
-      <c r="J22" t="s">
+      <c r="L22" t="s">
         <v>177</v>
       </c>
-      <c r="K22" t="s">
+      <c r="M22" t="s">
         <v>378</v>
       </c>
-      <c r="L22" t="s">
+      <c r="N22" t="s">
         <v>399</v>
       </c>
-      <c r="M22" t="s">
+      <c r="O22" t="s">
         <v>427</v>
       </c>
-      <c r="N22" t="s">
+      <c r="P22" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>96</v>
       </c>
@@ -3079,28 +3417,34 @@
         <v>120</v>
       </c>
       <c r="H23" t="s">
+        <v>100</v>
+      </c>
+      <c r="I23" t="s">
+        <v>621</v>
+      </c>
+      <c r="J23" t="s">
         <v>319</v>
       </c>
-      <c r="I23" t="s">
+      <c r="K23" t="s">
         <v>54</v>
       </c>
-      <c r="J23" t="s">
+      <c r="L23" t="s">
         <v>173</v>
       </c>
-      <c r="K23" t="s">
+      <c r="M23" t="s">
         <v>201</v>
       </c>
-      <c r="L23" t="s">
+      <c r="N23" t="s">
         <v>221</v>
       </c>
-      <c r="M23" t="s">
+      <c r="O23" t="s">
         <v>428</v>
       </c>
-      <c r="N23" t="s">
+      <c r="P23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>192</v>
       </c>
@@ -3123,28 +3467,34 @@
         <v>10</v>
       </c>
       <c r="H24" t="s">
-        <v>198</v>
+        <v>255</v>
       </c>
       <c r="I24" t="s">
-        <v>20</v>
+        <v>330</v>
       </c>
       <c r="J24" t="s">
         <v>198</v>
       </c>
       <c r="K24" t="s">
+        <v>20</v>
+      </c>
+      <c r="L24" t="s">
+        <v>198</v>
+      </c>
+      <c r="M24" t="s">
         <v>78</v>
       </c>
-      <c r="L24" t="s">
+      <c r="N24" t="s">
         <v>152</v>
       </c>
-      <c r="M24" t="s">
+      <c r="O24" t="s">
         <v>425</v>
       </c>
-      <c r="N24" t="s">
+      <c r="P24" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>336</v>
       </c>
@@ -3167,28 +3517,34 @@
         <v>111</v>
       </c>
       <c r="H25" t="s">
-        <v>320</v>
+        <v>581</v>
       </c>
       <c r="I25" t="s">
         <v>26</v>
       </c>
       <c r="J25" t="s">
+        <v>320</v>
+      </c>
+      <c r="K25" t="s">
+        <v>26</v>
+      </c>
+      <c r="L25" t="s">
         <v>199</v>
       </c>
-      <c r="K25" t="s">
+      <c r="M25" t="s">
         <v>373</v>
       </c>
-      <c r="L25" t="s">
+      <c r="N25" t="s">
         <v>206</v>
       </c>
-      <c r="M25" t="s">
+      <c r="O25" t="s">
         <v>223</v>
       </c>
-      <c r="N25" t="s">
+      <c r="P25" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>720</v>
       </c>
@@ -3211,28 +3567,34 @@
         <v>259</v>
       </c>
       <c r="H26" t="s">
+        <v>582</v>
+      </c>
+      <c r="I26" t="s">
+        <v>622</v>
+      </c>
+      <c r="J26" t="s">
         <v>321</v>
       </c>
-      <c r="I26" t="s">
+      <c r="K26" t="s">
         <v>55</v>
       </c>
-      <c r="J26" t="s">
+      <c r="L26" t="s">
         <v>200</v>
       </c>
-      <c r="K26" t="s">
+      <c r="M26" t="s">
         <v>379</v>
       </c>
-      <c r="L26" t="s">
+      <c r="N26" t="s">
         <v>400</v>
       </c>
-      <c r="M26" t="s">
+      <c r="O26" t="s">
         <v>429</v>
       </c>
-      <c r="N26" t="s">
+      <c r="P26" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>24</v>
       </c>
@@ -3255,28 +3617,34 @@
         <v>159</v>
       </c>
       <c r="H27" t="s">
+        <v>369</v>
+      </c>
+      <c r="I27" t="s">
+        <v>158</v>
+      </c>
+      <c r="J27" t="s">
         <v>329</v>
       </c>
-      <c r="I27" t="s">
+      <c r="K27" t="s">
         <v>56</v>
       </c>
-      <c r="J27" t="s">
+      <c r="L27" t="s">
         <v>145</v>
       </c>
-      <c r="K27" t="s">
+      <c r="M27" t="s">
         <v>380</v>
       </c>
-      <c r="L27" t="s">
+      <c r="N27" t="s">
         <v>264</v>
       </c>
-      <c r="M27" t="s">
+      <c r="O27" t="s">
         <v>480</v>
       </c>
-      <c r="N27" t="s">
+      <c r="P27" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>96</v>
       </c>
@@ -3299,28 +3667,34 @@
         <v>160</v>
       </c>
       <c r="H28" t="s">
+        <v>506</v>
+      </c>
+      <c r="I28" t="s">
+        <v>104</v>
+      </c>
+      <c r="J28" t="s">
         <v>330</v>
       </c>
-      <c r="I28" t="s">
+      <c r="K28" t="s">
         <v>57</v>
       </c>
-      <c r="J28" t="s">
+      <c r="L28" t="s">
         <v>201</v>
       </c>
-      <c r="K28" t="s">
+      <c r="M28" t="s">
         <v>381</v>
       </c>
-      <c r="L28" t="s">
+      <c r="N28" t="s">
         <v>319</v>
       </c>
-      <c r="M28" t="s">
+      <c r="O28" t="s">
         <v>481</v>
       </c>
-      <c r="N28" t="s">
+      <c r="P28" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>192</v>
       </c>
@@ -3343,28 +3717,34 @@
         <v>141</v>
       </c>
       <c r="H29" t="s">
+        <v>382</v>
+      </c>
+      <c r="I29" t="s">
+        <v>505</v>
+      </c>
+      <c r="J29" t="s">
         <v>121</v>
       </c>
-      <c r="I29" t="s">
+      <c r="K29" t="s">
         <v>58</v>
       </c>
-      <c r="J29" t="s">
+      <c r="L29" t="s">
         <v>124</v>
       </c>
-      <c r="K29" t="s">
+      <c r="M29" t="s">
         <v>185</v>
       </c>
-      <c r="L29" t="s">
+      <c r="N29" t="s">
         <v>138</v>
       </c>
-      <c r="M29" t="s">
+      <c r="O29" t="s">
         <v>13</v>
       </c>
-      <c r="N29" t="s">
+      <c r="P29" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>336</v>
       </c>
@@ -3387,28 +3767,34 @@
         <v>161</v>
       </c>
       <c r="H30" t="s">
+        <v>384</v>
+      </c>
+      <c r="I30" t="s">
+        <v>109</v>
+      </c>
+      <c r="J30" t="s">
         <v>125</v>
       </c>
-      <c r="I30" t="s">
+      <c r="K30" t="s">
         <v>59</v>
       </c>
-      <c r="J30" t="s">
+      <c r="L30" t="s">
         <v>184</v>
       </c>
-      <c r="K30" t="s">
+      <c r="M30" t="s">
         <v>161</v>
       </c>
-      <c r="L30" t="s">
+      <c r="N30" t="s">
         <v>285</v>
       </c>
-      <c r="M30" t="s">
+      <c r="O30" t="s">
         <v>184</v>
       </c>
-      <c r="N30" t="s">
+      <c r="P30" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>720</v>
       </c>
@@ -3431,28 +3817,34 @@
         <v>162</v>
       </c>
       <c r="H31" t="s">
+        <v>11</v>
+      </c>
+      <c r="I31" t="s">
+        <v>623</v>
+      </c>
+      <c r="J31" t="s">
         <v>331</v>
       </c>
-      <c r="I31" t="s">
+      <c r="K31" t="s">
         <v>60</v>
       </c>
-      <c r="J31" t="s">
+      <c r="L31" t="s">
         <v>106</v>
       </c>
-      <c r="K31" t="s">
+      <c r="M31" t="s">
         <v>382</v>
       </c>
-      <c r="L31" t="s">
+      <c r="N31" t="s">
         <v>207</v>
       </c>
-      <c r="M31" t="s">
+      <c r="O31" t="s">
         <v>139</v>
       </c>
-      <c r="N31" t="s">
+      <c r="P31" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>24</v>
       </c>
@@ -3475,28 +3867,34 @@
         <v>130</v>
       </c>
       <c r="H32" t="s">
+        <v>583</v>
+      </c>
+      <c r="I32" t="s">
+        <v>624</v>
+      </c>
+      <c r="J32" t="s">
         <v>332</v>
       </c>
-      <c r="I32" t="s">
+      <c r="K32" t="s">
         <v>61</v>
       </c>
-      <c r="J32" t="s">
+      <c r="L32" t="s">
         <v>202</v>
       </c>
-      <c r="K32" t="s">
+      <c r="M32" t="s">
         <v>358</v>
       </c>
-      <c r="L32" t="s">
+      <c r="N32" t="s">
         <v>410</v>
       </c>
-      <c r="M32" t="s">
+      <c r="O32" t="s">
         <v>430</v>
       </c>
-      <c r="N32" t="s">
+      <c r="P32" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>36</v>
       </c>
@@ -3519,28 +3917,34 @@
         <v>260</v>
       </c>
       <c r="H33" t="s">
+        <v>585</v>
+      </c>
+      <c r="I33" t="s">
+        <v>625</v>
+      </c>
+      <c r="J33" t="s">
         <v>333</v>
       </c>
-      <c r="I33" t="s">
+      <c r="K33" t="s">
         <v>62</v>
       </c>
-      <c r="J33" t="s">
+      <c r="L33" t="s">
         <v>203</v>
       </c>
-      <c r="K33" t="s">
+      <c r="M33" t="s">
         <v>359</v>
       </c>
-      <c r="L33" t="s">
+      <c r="N33" t="s">
         <v>411</v>
       </c>
-      <c r="M33" t="s">
+      <c r="O33" t="s">
         <v>431</v>
       </c>
-      <c r="N33" t="s">
+      <c r="P33" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>48</v>
       </c>
@@ -3563,28 +3967,34 @@
         <v>261</v>
       </c>
       <c r="H34" t="s">
+        <v>586</v>
+      </c>
+      <c r="I34" t="s">
+        <v>626</v>
+      </c>
+      <c r="J34" t="s">
         <v>334</v>
       </c>
-      <c r="I34" t="s">
+      <c r="K34" t="s">
         <v>63</v>
       </c>
-      <c r="J34" t="s">
+      <c r="L34" t="s">
         <v>204</v>
       </c>
-      <c r="K34" t="s">
+      <c r="M34" t="s">
         <v>360</v>
       </c>
-      <c r="L34" t="s">
+      <c r="N34" t="s">
         <v>412</v>
       </c>
-      <c r="M34" t="s">
+      <c r="O34" t="s">
         <v>432</v>
       </c>
-      <c r="N34" t="s">
+      <c r="P34" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>60</v>
       </c>
@@ -3607,28 +4017,34 @@
         <v>187</v>
       </c>
       <c r="H35" t="s">
+        <v>271</v>
+      </c>
+      <c r="I35" t="s">
+        <v>627</v>
+      </c>
+      <c r="J35" t="s">
         <v>335</v>
       </c>
-      <c r="I35" t="s">
+      <c r="K35" t="s">
         <v>64</v>
       </c>
-      <c r="J35" t="s">
+      <c r="L35" t="s">
         <v>183</v>
       </c>
-      <c r="K35" t="s">
+      <c r="M35" t="s">
         <v>361</v>
       </c>
-      <c r="L35" t="s">
+      <c r="N35" t="s">
         <v>413</v>
       </c>
-      <c r="M35" t="s">
+      <c r="O35" t="s">
         <v>204</v>
       </c>
-      <c r="N35" t="s">
+      <c r="P35" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>24</v>
       </c>
@@ -3651,28 +4067,34 @@
         <v>560</v>
       </c>
       <c r="H36" t="s">
+        <v>587</v>
+      </c>
+      <c r="I36" t="s">
+        <v>628</v>
+      </c>
+      <c r="J36" t="s">
         <v>514</v>
       </c>
-      <c r="I36" t="s">
+      <c r="K36" t="s">
         <v>525</v>
       </c>
-      <c r="J36" t="s">
+      <c r="L36" t="s">
         <v>329</v>
       </c>
-      <c r="K36" t="s">
+      <c r="M36" t="s">
         <v>79</v>
       </c>
-      <c r="L36" t="s">
+      <c r="N36" t="s">
         <v>496</v>
       </c>
-      <c r="M36" t="s">
+      <c r="O36" t="s">
         <v>398</v>
       </c>
-      <c r="N36" t="s">
+      <c r="P36" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3695,28 +4117,34 @@
         <v>561</v>
       </c>
       <c r="H37" t="s">
+        <v>588</v>
+      </c>
+      <c r="I37" t="s">
+        <v>629</v>
+      </c>
+      <c r="J37" t="s">
         <v>517</v>
       </c>
-      <c r="I37" t="s">
+      <c r="K37" t="s">
         <v>497</v>
       </c>
-      <c r="J37" t="s">
+      <c r="L37" t="s">
         <v>54</v>
       </c>
-      <c r="K37" t="s">
+      <c r="M37" t="s">
         <v>488</v>
       </c>
-      <c r="L37" t="s">
+      <c r="N37" t="s">
         <v>497</v>
       </c>
-      <c r="M37" t="s">
+      <c r="O37" t="s">
         <v>485</v>
       </c>
-      <c r="N37" t="s">
+      <c r="P37" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>48</v>
       </c>
@@ -3739,28 +4167,34 @@
         <v>562</v>
       </c>
       <c r="H38" t="s">
+        <v>539</v>
+      </c>
+      <c r="I38" t="s">
+        <v>76</v>
+      </c>
+      <c r="J38" t="s">
         <v>516</v>
       </c>
-      <c r="I38" t="s">
+      <c r="K38" t="s">
         <v>526</v>
       </c>
-      <c r="J38" t="s">
+      <c r="L38" t="s">
         <v>12</v>
       </c>
-      <c r="K38" t="s">
+      <c r="M38" t="s">
         <v>286</v>
       </c>
-      <c r="L38" t="s">
+      <c r="N38" t="s">
         <v>498</v>
       </c>
-      <c r="M38" t="s">
+      <c r="O38" t="s">
         <v>139</v>
       </c>
-      <c r="N38" t="s">
+      <c r="P38" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>60</v>
       </c>
@@ -3783,28 +4217,34 @@
         <v>563</v>
       </c>
       <c r="H39" t="s">
+        <v>589</v>
+      </c>
+      <c r="I39" t="s">
+        <v>630</v>
+      </c>
+      <c r="J39" t="s">
         <v>515</v>
       </c>
-      <c r="I39" t="s">
+      <c r="K39" t="s">
         <v>527</v>
       </c>
-      <c r="J39" t="s">
+      <c r="L39" t="s">
         <v>116</v>
       </c>
-      <c r="K39" t="s">
+      <c r="M39" t="s">
         <v>489</v>
       </c>
-      <c r="L39" t="s">
+      <c r="N39" t="s">
         <v>499</v>
       </c>
-      <c r="M39" t="s">
+      <c r="O39" t="s">
         <v>265</v>
       </c>
-      <c r="N39" t="s">
+      <c r="P39" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>24</v>
       </c>
@@ -3827,28 +4267,34 @@
         <v>564</v>
       </c>
       <c r="H40" t="s">
+        <v>516</v>
+      </c>
+      <c r="I40" t="s">
+        <v>212</v>
+      </c>
+      <c r="J40" t="s">
         <v>509</v>
       </c>
-      <c r="I40" t="s">
+      <c r="K40" t="s">
         <v>528</v>
       </c>
-      <c r="J40" t="s">
+      <c r="L40" t="s">
         <v>390</v>
       </c>
-      <c r="K40" t="s">
+      <c r="M40" t="s">
         <v>385</v>
       </c>
-      <c r="L40" t="s">
+      <c r="N40" t="s">
         <v>160</v>
       </c>
-      <c r="M40" t="s">
+      <c r="O40" t="s">
         <v>371</v>
       </c>
-      <c r="N40" t="s">
+      <c r="P40" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>96</v>
       </c>
@@ -3871,28 +4317,34 @@
         <v>329</v>
       </c>
       <c r="H41" t="s">
+        <v>514</v>
+      </c>
+      <c r="I41" t="s">
+        <v>105</v>
+      </c>
+      <c r="J41" t="s">
         <v>510</v>
       </c>
-      <c r="I41" t="s">
+      <c r="K41" t="s">
         <v>529</v>
       </c>
-      <c r="J41" t="s">
+      <c r="L41" t="s">
         <v>19</v>
       </c>
-      <c r="K41" t="s">
+      <c r="M41" t="s">
         <v>490</v>
       </c>
-      <c r="L41" t="s">
+      <c r="N41" t="s">
         <v>170</v>
       </c>
-      <c r="M41" t="s">
+      <c r="O41" t="s">
         <v>426</v>
       </c>
-      <c r="N41" t="s">
+      <c r="P41" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>192</v>
       </c>
@@ -3915,28 +4367,34 @@
         <v>124</v>
       </c>
       <c r="H42" t="s">
+        <v>590</v>
+      </c>
+      <c r="I42" t="s">
+        <v>181</v>
+      </c>
+      <c r="J42" t="s">
         <v>511</v>
       </c>
-      <c r="I42" t="s">
+      <c r="K42" t="s">
         <v>78</v>
       </c>
-      <c r="J42" t="s">
+      <c r="L42" t="s">
         <v>233</v>
       </c>
-      <c r="K42" t="s">
+      <c r="M42" t="s">
         <v>276</v>
       </c>
-      <c r="L42" t="s">
+      <c r="N42" t="s">
         <v>105</v>
       </c>
-      <c r="M42" t="s">
+      <c r="O42" t="s">
         <v>425</v>
       </c>
-      <c r="N42" t="s">
+      <c r="P42" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>336</v>
       </c>
@@ -3959,28 +4417,34 @@
         <v>19</v>
       </c>
       <c r="H43" t="s">
+        <v>591</v>
+      </c>
+      <c r="I43" t="s">
+        <v>372</v>
+      </c>
+      <c r="J43" t="s">
         <v>512</v>
       </c>
-      <c r="I43" t="s">
+      <c r="K43" t="s">
         <v>152</v>
       </c>
-      <c r="J43" t="s">
+      <c r="L43" t="s">
         <v>106</v>
       </c>
-      <c r="K43" t="s">
+      <c r="M43" t="s">
         <v>372</v>
       </c>
-      <c r="L43" t="s">
+      <c r="N43" t="s">
         <v>88</v>
       </c>
-      <c r="M43" t="s">
+      <c r="O43" t="s">
         <v>384</v>
       </c>
-      <c r="N43" t="s">
+      <c r="P43" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>720</v>
       </c>
@@ -4003,28 +4467,34 @@
         <v>171</v>
       </c>
       <c r="H44" t="s">
+        <v>592</v>
+      </c>
+      <c r="I44" t="s">
+        <v>327</v>
+      </c>
+      <c r="J44" t="s">
         <v>513</v>
       </c>
-      <c r="I44" t="s">
+      <c r="K44" t="s">
         <v>11</v>
       </c>
-      <c r="J44" t="s">
+      <c r="L44" t="s">
         <v>192</v>
       </c>
-      <c r="K44" t="s">
+      <c r="M44" t="s">
         <v>155</v>
       </c>
-      <c r="L44" t="s">
+      <c r="N44" t="s">
         <v>93</v>
       </c>
-      <c r="M44" t="s">
+      <c r="O44" t="s">
         <v>73</v>
       </c>
-      <c r="N44" t="s">
+      <c r="P44" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>24</v>
       </c>
@@ -4047,28 +4517,34 @@
         <v>181</v>
       </c>
       <c r="H45" t="s">
+        <v>593</v>
+      </c>
+      <c r="I45" t="s">
+        <v>401</v>
+      </c>
+      <c r="J45" t="s">
         <v>336</v>
       </c>
-      <c r="I45" t="s">
+      <c r="K45" t="s">
         <v>72</v>
       </c>
-      <c r="J45" t="s">
+      <c r="L45" t="s">
         <v>83</v>
       </c>
-      <c r="K45" t="s">
+      <c r="M45" t="s">
         <v>383</v>
       </c>
-      <c r="L45" t="s">
+      <c r="N45" t="s">
         <v>401</v>
       </c>
-      <c r="M45" t="s">
+      <c r="O45" t="s">
         <v>162</v>
       </c>
-      <c r="N45" t="s">
+      <c r="P45" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>96</v>
       </c>
@@ -4091,28 +4567,34 @@
         <v>163</v>
       </c>
       <c r="H46" t="s">
+        <v>63</v>
+      </c>
+      <c r="I46" t="s">
+        <v>47</v>
+      </c>
+      <c r="J46" t="s">
         <v>337</v>
       </c>
-      <c r="I46" t="s">
+      <c r="K46" t="s">
         <v>73</v>
       </c>
-      <c r="J46" t="s">
+      <c r="L46" t="s">
         <v>135</v>
       </c>
-      <c r="K46" t="s">
+      <c r="M46" t="s">
         <v>226</v>
       </c>
-      <c r="L46" t="s">
+      <c r="N46" t="s">
         <v>224</v>
       </c>
-      <c r="M46" t="s">
+      <c r="O46" t="s">
         <v>195</v>
       </c>
-      <c r="N46" t="s">
+      <c r="P46" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>192</v>
       </c>
@@ -4135,28 +4617,34 @@
         <v>164</v>
       </c>
       <c r="H47" t="s">
+        <v>594</v>
+      </c>
+      <c r="I47" t="s">
+        <v>115</v>
+      </c>
+      <c r="J47" t="s">
         <v>338</v>
       </c>
-      <c r="I47" t="s">
+      <c r="K47" t="s">
         <v>74</v>
       </c>
-      <c r="J47" t="s">
+      <c r="L47" t="s">
         <v>26</v>
       </c>
-      <c r="K47" t="s">
+      <c r="M47" t="s">
         <v>367</v>
       </c>
-      <c r="L47" t="s">
+      <c r="N47" t="s">
         <v>374</v>
       </c>
-      <c r="M47" t="s">
+      <c r="O47" t="s">
         <v>114</v>
       </c>
-      <c r="N47" t="s">
+      <c r="P47" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>336</v>
       </c>
@@ -4179,28 +4667,34 @@
         <v>262</v>
       </c>
       <c r="H48" t="s">
+        <v>595</v>
+      </c>
+      <c r="I48" t="s">
+        <v>629</v>
+      </c>
+      <c r="J48" t="s">
         <v>339</v>
       </c>
-      <c r="I48" t="s">
+      <c r="K48" t="s">
         <v>75</v>
       </c>
-      <c r="J48" t="s">
+      <c r="L48" t="s">
         <v>205</v>
       </c>
-      <c r="K48" t="s">
+      <c r="M48" t="s">
         <v>374</v>
       </c>
-      <c r="L48" t="s">
+      <c r="N48" t="s">
         <v>283</v>
       </c>
-      <c r="M48" t="s">
+      <c r="O48" t="s">
         <v>11</v>
       </c>
-      <c r="N48" t="s">
+      <c r="P48" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>720</v>
       </c>
@@ -4223,28 +4717,34 @@
         <v>263</v>
       </c>
       <c r="H49" t="s">
+        <v>64</v>
+      </c>
+      <c r="I49" t="s">
+        <v>631</v>
+      </c>
+      <c r="J49" t="s">
         <v>340</v>
       </c>
-      <c r="I49" t="s">
+      <c r="K49" t="s">
         <v>76</v>
       </c>
-      <c r="J49" t="s">
+      <c r="L49" t="s">
         <v>206</v>
       </c>
-      <c r="K49" t="s">
+      <c r="M49" t="s">
         <v>234</v>
       </c>
-      <c r="L49" t="s">
+      <c r="N49" t="s">
         <v>209</v>
       </c>
-      <c r="M49" t="s">
+      <c r="O49" t="s">
         <v>206</v>
       </c>
-      <c r="N49" t="s">
+      <c r="P49" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>24</v>
       </c>
@@ -4267,28 +4767,34 @@
         <v>264</v>
       </c>
       <c r="H50" t="s">
+        <v>596</v>
+      </c>
+      <c r="I50" t="s">
+        <v>371</v>
+      </c>
+      <c r="J50" t="s">
         <v>143</v>
       </c>
-      <c r="I50" t="s">
+      <c r="K50" t="s">
         <v>77</v>
       </c>
-      <c r="J50" t="s">
+      <c r="L50" t="s">
         <v>127</v>
       </c>
-      <c r="K50" t="s">
+      <c r="M50" t="s">
         <v>385</v>
       </c>
-      <c r="L50" t="s">
+      <c r="N50" t="s">
         <v>201</v>
       </c>
-      <c r="M50" t="s">
+      <c r="O50" t="s">
         <v>433</v>
       </c>
-      <c r="N50" t="s">
+      <c r="P50" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>96</v>
       </c>
@@ -4311,28 +4817,34 @@
         <v>104</v>
       </c>
       <c r="H51" t="s">
+        <v>188</v>
+      </c>
+      <c r="I51" t="s">
+        <v>131</v>
+      </c>
+      <c r="J51" t="s">
         <v>341</v>
       </c>
-      <c r="I51" t="s">
+      <c r="K51" t="s">
         <v>78</v>
       </c>
-      <c r="J51" t="s">
+      <c r="L51" t="s">
         <v>194</v>
       </c>
-      <c r="K51" t="s">
+      <c r="M51" t="s">
         <v>14</v>
       </c>
-      <c r="L51" t="s">
+      <c r="N51" t="s">
         <v>100</v>
       </c>
-      <c r="M51" t="s">
+      <c r="O51" t="s">
         <v>138</v>
       </c>
-      <c r="N51" t="s">
+      <c r="P51" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>192</v>
       </c>
@@ -4355,28 +4867,34 @@
         <v>227</v>
       </c>
       <c r="H52" t="s">
+        <v>597</v>
+      </c>
+      <c r="I52" t="s">
+        <v>553</v>
+      </c>
+      <c r="J52" t="s">
         <v>244</v>
       </c>
-      <c r="I52" t="s">
+      <c r="K52" t="s">
         <v>79</v>
       </c>
-      <c r="J52" t="s">
+      <c r="L52" t="s">
         <v>207</v>
       </c>
-      <c r="K52" t="s">
+      <c r="M52" t="s">
         <v>198</v>
       </c>
-      <c r="L52" t="s">
+      <c r="N52" t="s">
         <v>45</v>
       </c>
-      <c r="M52" t="s">
+      <c r="O52" t="s">
         <v>401</v>
       </c>
-      <c r="N52" t="s">
+      <c r="P52" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>336</v>
       </c>
@@ -4399,28 +4917,34 @@
         <v>142</v>
       </c>
       <c r="H53" t="s">
+        <v>598</v>
+      </c>
+      <c r="I53" t="s">
+        <v>632</v>
+      </c>
+      <c r="J53" t="s">
         <v>36</v>
       </c>
-      <c r="I53" t="s">
+      <c r="K53" t="s">
         <v>80</v>
       </c>
-      <c r="J53" t="s">
+      <c r="L53" t="s">
         <v>152</v>
       </c>
-      <c r="K53" t="s">
+      <c r="M53" t="s">
         <v>121</v>
       </c>
-      <c r="L53" t="s">
+      <c r="N53" t="s">
         <v>51</v>
       </c>
-      <c r="M53" t="s">
+      <c r="O53" t="s">
         <v>129</v>
       </c>
-      <c r="N53" t="s">
+      <c r="P53" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>720</v>
       </c>
@@ -4443,28 +4967,34 @@
         <v>166</v>
       </c>
       <c r="H54" t="s">
+        <v>599</v>
+      </c>
+      <c r="I54" t="s">
         <v>44</v>
       </c>
-      <c r="I54" t="s">
+      <c r="J54" t="s">
+        <v>44</v>
+      </c>
+      <c r="K54" t="s">
         <v>81</v>
       </c>
-      <c r="J54" t="s">
+      <c r="L54" t="s">
         <v>101</v>
       </c>
-      <c r="K54" t="s">
+      <c r="M54" t="s">
         <v>352</v>
       </c>
-      <c r="L54" t="s">
+      <c r="N54" t="s">
         <v>166</v>
       </c>
-      <c r="M54" t="s">
+      <c r="O54" t="s">
         <v>327</v>
       </c>
-      <c r="N54" t="s">
+      <c r="P54" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>24</v>
       </c>
@@ -4487,28 +5017,34 @@
         <v>99</v>
       </c>
       <c r="H55" t="s">
+        <v>600</v>
+      </c>
+      <c r="I55" t="s">
+        <v>221</v>
+      </c>
+      <c r="J55" t="s">
         <v>342</v>
       </c>
-      <c r="I55" t="s">
+      <c r="K55" t="s">
         <v>82</v>
       </c>
-      <c r="J55" t="s">
+      <c r="L55" t="s">
         <v>34</v>
       </c>
-      <c r="K55" t="s">
+      <c r="M55" t="s">
         <v>169</v>
       </c>
-      <c r="L55" t="s">
+      <c r="N55" t="s">
         <v>124</v>
       </c>
-      <c r="M55" t="s">
+      <c r="O55" t="s">
         <v>146</v>
       </c>
-      <c r="N55" t="s">
+      <c r="P55" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>96</v>
       </c>
@@ -4531,28 +5067,34 @@
         <v>265</v>
       </c>
       <c r="H56" t="s">
+        <v>601</v>
+      </c>
+      <c r="I56" t="s">
+        <v>21</v>
+      </c>
+      <c r="J56" t="s">
         <v>343</v>
       </c>
-      <c r="I56" t="s">
+      <c r="K56" t="s">
         <v>83</v>
       </c>
-      <c r="J56" t="s">
+      <c r="L56" t="s">
         <v>181</v>
       </c>
-      <c r="K56" t="s">
+      <c r="M56" t="s">
         <v>20</v>
       </c>
-      <c r="L56" t="s">
+      <c r="N56" t="s">
         <v>402</v>
       </c>
-      <c r="M56" t="s">
+      <c r="O56" t="s">
         <v>341</v>
       </c>
-      <c r="N56" t="s">
+      <c r="P56" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>192</v>
       </c>
@@ -4575,28 +5117,34 @@
         <v>266</v>
       </c>
       <c r="H57" t="s">
+        <v>602</v>
+      </c>
+      <c r="I57" t="s">
+        <v>157</v>
+      </c>
+      <c r="J57" t="s">
         <v>344</v>
       </c>
-      <c r="I57" t="s">
+      <c r="K57" t="s">
         <v>84</v>
       </c>
-      <c r="J57" t="s">
+      <c r="L57" t="s">
         <v>152</v>
       </c>
-      <c r="K57" t="s">
+      <c r="M57" t="s">
         <v>386</v>
       </c>
-      <c r="L57" t="s">
+      <c r="N57" t="s">
         <v>167</v>
       </c>
-      <c r="M57" t="s">
+      <c r="O57" t="s">
         <v>554</v>
       </c>
-      <c r="N57" t="s">
+      <c r="P57" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>336</v>
       </c>
@@ -4619,28 +5167,34 @@
         <v>84</v>
       </c>
       <c r="H58" t="s">
+        <v>64</v>
+      </c>
+      <c r="I58" t="s">
+        <v>73</v>
+      </c>
+      <c r="J58" t="s">
         <v>271</v>
       </c>
-      <c r="I58" t="s">
+      <c r="K58" t="s">
         <v>42</v>
       </c>
-      <c r="J58" t="s">
+      <c r="L58" t="s">
         <v>208</v>
       </c>
-      <c r="K58" t="s">
+      <c r="M58" t="s">
         <v>387</v>
       </c>
-      <c r="L58" t="s">
+      <c r="N58" t="s">
         <v>46</v>
       </c>
-      <c r="M58" t="s">
+      <c r="O58" t="s">
         <v>166</v>
       </c>
-      <c r="N58" t="s">
+      <c r="P58" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>720</v>
       </c>
@@ -4663,28 +5217,34 @@
         <v>225</v>
       </c>
       <c r="H59" t="s">
+        <v>603</v>
+      </c>
+      <c r="I59" t="s">
+        <v>630</v>
+      </c>
+      <c r="J59" t="s">
         <v>249</v>
       </c>
-      <c r="I59" t="s">
+      <c r="K59" t="s">
         <v>38</v>
       </c>
-      <c r="J59" t="s">
+      <c r="L59" t="s">
         <v>209</v>
       </c>
-      <c r="K59" t="s">
+      <c r="M59" t="s">
         <v>205</v>
       </c>
-      <c r="L59" t="s">
+      <c r="N59" t="s">
         <v>403</v>
       </c>
-      <c r="M59" t="s">
+      <c r="O59" t="s">
         <v>36</v>
       </c>
-      <c r="N59" t="s">
+      <c r="P59" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>24</v>
       </c>
@@ -4707,28 +5267,34 @@
         <v>16</v>
       </c>
       <c r="H60" t="s">
+        <v>604</v>
+      </c>
+      <c r="I60" t="s">
+        <v>178</v>
+      </c>
+      <c r="J60" t="s">
         <v>345</v>
       </c>
-      <c r="I60" t="s">
+      <c r="K60" t="s">
         <v>85</v>
       </c>
-      <c r="J60" t="s">
+      <c r="L60" t="s">
         <v>210</v>
       </c>
-      <c r="K60" t="s">
+      <c r="M60" t="s">
         <v>388</v>
       </c>
-      <c r="L60" t="s">
+      <c r="N60" t="s">
         <v>107</v>
       </c>
-      <c r="M60" t="s">
+      <c r="O60" t="s">
         <v>555</v>
       </c>
-      <c r="N60" t="s">
+      <c r="P60" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>96</v>
       </c>
@@ -4751,28 +5317,34 @@
         <v>211</v>
       </c>
       <c r="H61" t="s">
+        <v>467</v>
+      </c>
+      <c r="I61" t="s">
+        <v>160</v>
+      </c>
+      <c r="J61" t="s">
         <v>12</v>
       </c>
-      <c r="I61" t="s">
+      <c r="K61" t="s">
         <v>86</v>
       </c>
-      <c r="J61" t="s">
+      <c r="L61" t="s">
         <v>211</v>
       </c>
-      <c r="K61" t="s">
+      <c r="M61" t="s">
         <v>389</v>
       </c>
-      <c r="L61" t="s">
+      <c r="N61" t="s">
         <v>404</v>
       </c>
-      <c r="M61" t="s">
+      <c r="O61" t="s">
         <v>556</v>
       </c>
-      <c r="N61" t="s">
+      <c r="P61" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>192</v>
       </c>
@@ -4795,28 +5367,34 @@
         <v>134</v>
       </c>
       <c r="H62" t="s">
-        <v>346</v>
+        <v>129</v>
       </c>
       <c r="I62" t="s">
         <v>87</v>
       </c>
       <c r="J62" t="s">
+        <v>346</v>
+      </c>
+      <c r="K62" t="s">
+        <v>87</v>
+      </c>
+      <c r="L62" t="s">
         <v>212</v>
       </c>
-      <c r="K62" t="s">
+      <c r="M62" t="s">
         <v>390</v>
       </c>
-      <c r="L62" t="s">
+      <c r="N62" t="s">
         <v>128</v>
       </c>
-      <c r="M62" t="s">
+      <c r="O62" t="s">
         <v>490</v>
       </c>
-      <c r="N62" t="s">
+      <c r="P62" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>336</v>
       </c>
@@ -4839,28 +5417,34 @@
         <v>161</v>
       </c>
       <c r="H63" t="s">
+        <v>84</v>
+      </c>
+      <c r="I63" t="s">
+        <v>256</v>
+      </c>
+      <c r="J63" t="s">
         <v>113</v>
       </c>
-      <c r="I63" t="s">
+      <c r="K63" t="s">
         <v>88</v>
       </c>
-      <c r="J63" t="s">
+      <c r="L63" t="s">
         <v>100</v>
       </c>
-      <c r="K63" t="s">
+      <c r="M63" t="s">
         <v>276</v>
       </c>
-      <c r="L63" t="s">
+      <c r="N63" t="s">
         <v>19</v>
       </c>
-      <c r="M63" t="s">
+      <c r="O63" t="s">
         <v>175</v>
       </c>
-      <c r="N63" t="s">
+      <c r="P63" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>720</v>
       </c>
@@ -4883,28 +5467,34 @@
         <v>267</v>
       </c>
       <c r="H64" t="s">
+        <v>605</v>
+      </c>
+      <c r="I64" t="s">
+        <v>331</v>
+      </c>
+      <c r="J64" t="s">
         <v>347</v>
       </c>
-      <c r="I64" t="s">
+      <c r="K64" t="s">
         <v>89</v>
       </c>
-      <c r="J64" t="s">
+      <c r="L64" t="s">
         <v>46</v>
       </c>
-      <c r="K64" t="s">
+      <c r="M64" t="s">
         <v>295</v>
       </c>
-      <c r="L64" t="s">
+      <c r="N64" t="s">
         <v>41</v>
       </c>
-      <c r="M64" t="s">
+      <c r="O64" t="s">
         <v>125</v>
       </c>
-      <c r="N64" t="s">
+      <c r="P64" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>24</v>
       </c>
@@ -4927,28 +5517,34 @@
         <v>182</v>
       </c>
       <c r="H65" t="s">
+        <v>392</v>
+      </c>
+      <c r="I65" t="s">
+        <v>633</v>
+      </c>
+      <c r="J65" t="s">
         <v>348</v>
       </c>
-      <c r="I65" t="s">
+      <c r="K65" t="s">
         <v>27</v>
       </c>
-      <c r="J65" t="s">
+      <c r="L65" t="s">
         <v>108</v>
-      </c>
-      <c r="K65" t="s">
-        <v>391</v>
-      </c>
-      <c r="L65" t="s">
-        <v>405</v>
       </c>
       <c r="M65" t="s">
         <v>391</v>
       </c>
       <c r="N65" t="s">
+        <v>405</v>
+      </c>
+      <c r="O65" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="P65" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>96</v>
       </c>
@@ -4971,28 +5567,34 @@
         <v>33</v>
       </c>
       <c r="H66" t="s">
+        <v>486</v>
+      </c>
+      <c r="I66" t="s">
+        <v>168</v>
+      </c>
+      <c r="J66" t="s">
         <v>349</v>
       </c>
-      <c r="I66" t="s">
+      <c r="K66" t="s">
         <v>90</v>
       </c>
-      <c r="J66" t="s">
+      <c r="L66" t="s">
         <v>213</v>
       </c>
-      <c r="K66" t="s">
+      <c r="M66" t="s">
         <v>392</v>
       </c>
-      <c r="L66" t="s">
+      <c r="N66" t="s">
         <v>406</v>
       </c>
-      <c r="M66" t="s">
+      <c r="O66" t="s">
         <v>434</v>
       </c>
-      <c r="N66" t="s">
+      <c r="P66" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>192</v>
       </c>
@@ -5015,28 +5617,34 @@
         <v>222</v>
       </c>
       <c r="H67" t="s">
-        <v>329</v>
+        <v>257</v>
       </c>
       <c r="I67" t="s">
         <v>86</v>
       </c>
       <c r="J67" t="s">
+        <v>329</v>
+      </c>
+      <c r="K67" t="s">
+        <v>86</v>
+      </c>
+      <c r="L67" t="s">
         <v>201</v>
       </c>
-      <c r="K67" t="s">
+      <c r="M67" t="s">
         <v>368</v>
       </c>
-      <c r="L67" t="s">
+      <c r="N67" t="s">
         <v>371</v>
       </c>
-      <c r="M67" t="s">
+      <c r="O67" t="s">
         <v>279</v>
       </c>
-      <c r="N67" t="s">
+      <c r="P67" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>336</v>
       </c>
@@ -5059,28 +5667,34 @@
         <v>268</v>
       </c>
       <c r="H68" t="s">
+        <v>228</v>
+      </c>
+      <c r="I68" t="s">
+        <v>372</v>
+      </c>
+      <c r="J68" t="s">
         <v>163</v>
       </c>
-      <c r="I68" t="s">
+      <c r="K68" t="s">
         <v>91</v>
       </c>
-      <c r="J68" t="s">
+      <c r="L68" t="s">
         <v>125</v>
       </c>
-      <c r="K68" t="s">
+      <c r="M68" t="s">
         <v>384</v>
       </c>
-      <c r="L68" t="s">
+      <c r="N68" t="s">
         <v>155</v>
       </c>
-      <c r="M68" t="s">
+      <c r="O68" t="s">
         <v>129</v>
       </c>
-      <c r="N68" t="s">
+      <c r="P68" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>720</v>
       </c>
@@ -5103,28 +5717,34 @@
         <v>269</v>
       </c>
       <c r="H69" t="s">
+        <v>606</v>
+      </c>
+      <c r="I69" t="s">
+        <v>64</v>
+      </c>
+      <c r="J69" t="s">
         <v>350</v>
       </c>
-      <c r="I69" t="s">
+      <c r="K69" t="s">
         <v>92</v>
       </c>
-      <c r="J69" t="s">
+      <c r="L69" t="s">
         <v>214</v>
       </c>
-      <c r="K69" t="s">
+      <c r="M69" t="s">
         <v>393</v>
       </c>
-      <c r="L69" t="s">
+      <c r="N69" t="s">
         <v>407</v>
       </c>
-      <c r="M69" t="s">
+      <c r="O69" t="s">
         <v>435</v>
       </c>
-      <c r="N69" t="s">
+      <c r="P69" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>24</v>
       </c>
@@ -5147,28 +5767,34 @@
         <v>168</v>
       </c>
       <c r="H70" t="s">
+        <v>173</v>
+      </c>
+      <c r="I70" t="s">
+        <v>406</v>
+      </c>
+      <c r="J70" t="s">
         <v>351</v>
       </c>
-      <c r="I70" t="s">
+      <c r="K70" t="s">
         <v>68</v>
       </c>
-      <c r="J70" t="s">
+      <c r="L70" t="s">
         <v>90</v>
       </c>
-      <c r="K70" t="s">
+      <c r="M70" t="s">
         <v>394</v>
       </c>
-      <c r="L70" t="s">
+      <c r="N70" t="s">
         <v>408</v>
       </c>
-      <c r="M70" t="s">
+      <c r="O70" t="s">
         <v>90</v>
       </c>
-      <c r="N70" t="s">
+      <c r="P70" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>96</v>
       </c>
@@ -5191,28 +5817,34 @@
         <v>243</v>
       </c>
       <c r="H71" t="s">
+        <v>369</v>
+      </c>
+      <c r="I71" t="s">
+        <v>368</v>
+      </c>
+      <c r="J71" t="s">
         <v>109</v>
       </c>
-      <c r="I71" t="s">
+      <c r="K71" t="s">
         <v>69</v>
       </c>
-      <c r="J71" t="s">
+      <c r="L71" t="s">
         <v>215</v>
       </c>
-      <c r="K71" t="s">
+      <c r="M71" t="s">
         <v>395</v>
       </c>
-      <c r="L71" t="s">
+      <c r="N71" t="s">
         <v>409</v>
       </c>
-      <c r="M71" t="s">
+      <c r="O71" t="s">
         <v>158</v>
       </c>
-      <c r="N71" t="s">
+      <c r="P71" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>192</v>
       </c>
@@ -5235,28 +5867,34 @@
         <v>169</v>
       </c>
       <c r="H72" t="s">
+        <v>233</v>
+      </c>
+      <c r="I72" t="s">
+        <v>490</v>
+      </c>
+      <c r="J72" t="s">
         <v>148</v>
       </c>
-      <c r="I72" t="s">
+      <c r="K72" t="s">
         <v>12</v>
       </c>
-      <c r="J72" t="s">
+      <c r="L72" t="s">
         <v>180</v>
       </c>
-      <c r="K72" t="s">
+      <c r="M72" t="s">
         <v>375</v>
       </c>
-      <c r="L72" t="s">
+      <c r="N72" t="s">
         <v>147</v>
       </c>
-      <c r="M72" t="s">
+      <c r="O72" t="s">
         <v>180</v>
       </c>
-      <c r="N72" t="s">
+      <c r="P72" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>336</v>
       </c>
@@ -5279,28 +5917,34 @@
         <v>170</v>
       </c>
       <c r="H73" t="s">
+        <v>295</v>
+      </c>
+      <c r="I73" t="s">
+        <v>383</v>
+      </c>
+      <c r="J73" t="s">
         <v>352</v>
       </c>
-      <c r="I73" t="s">
+      <c r="K73" t="s">
         <v>70</v>
       </c>
-      <c r="J73" t="s">
+      <c r="L73" t="s">
         <v>151</v>
       </c>
-      <c r="K73" t="s">
+      <c r="M73" t="s">
         <v>116</v>
       </c>
-      <c r="L73" t="s">
+      <c r="N73" t="s">
         <v>369</v>
       </c>
-      <c r="M73" t="s">
+      <c r="O73" t="s">
         <v>482</v>
       </c>
-      <c r="N73" t="s">
+      <c r="P73" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>720</v>
       </c>
@@ -5323,28 +5967,34 @@
         <v>171</v>
       </c>
       <c r="H74" t="s">
-        <v>328</v>
+        <v>370</v>
       </c>
       <c r="I74" t="s">
         <v>71</v>
       </c>
       <c r="J74" t="s">
-        <v>156</v>
+        <v>328</v>
       </c>
       <c r="K74" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="L74" t="s">
         <v>156</v>
       </c>
       <c r="M74" t="s">
+        <v>51</v>
+      </c>
+      <c r="N74" t="s">
+        <v>156</v>
+      </c>
+      <c r="O74" t="s">
         <v>21</v>
       </c>
-      <c r="N74" t="s">
+      <c r="P74" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>24</v>
       </c>
@@ -5367,28 +6017,34 @@
         <v>270</v>
       </c>
       <c r="H75" t="s">
+        <v>607</v>
+      </c>
+      <c r="I75" t="s">
+        <v>634</v>
+      </c>
+      <c r="J75" t="s">
         <v>353</v>
       </c>
-      <c r="I75" t="s">
+      <c r="K75" t="s">
         <v>67</v>
       </c>
-      <c r="J75" t="s">
+      <c r="L75" t="s">
         <v>216</v>
       </c>
-      <c r="K75" t="s">
+      <c r="M75" t="s">
         <v>362</v>
       </c>
-      <c r="L75" t="s">
+      <c r="N75" t="s">
         <v>414</v>
       </c>
-      <c r="M75" t="s">
+      <c r="O75" t="s">
         <v>436</v>
       </c>
-      <c r="N75" t="s">
+      <c r="P75" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>36</v>
       </c>
@@ -5411,28 +6067,34 @@
         <v>271</v>
       </c>
       <c r="H76" t="s">
+        <v>608</v>
+      </c>
+      <c r="I76" t="s">
+        <v>635</v>
+      </c>
+      <c r="J76" t="s">
         <v>354</v>
       </c>
-      <c r="I76" t="s">
+      <c r="K76" t="s">
         <v>65</v>
       </c>
-      <c r="J76" t="s">
+      <c r="L76" t="s">
         <v>217</v>
       </c>
-      <c r="K76" t="s">
+      <c r="M76" t="s">
         <v>363</v>
       </c>
-      <c r="L76" t="s">
+      <c r="N76" t="s">
         <v>415</v>
       </c>
-      <c r="M76" t="s">
+      <c r="O76" t="s">
         <v>437</v>
       </c>
-      <c r="N76" t="s">
+      <c r="P76" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>48</v>
       </c>
@@ -5455,28 +6117,34 @@
         <v>272</v>
       </c>
       <c r="H77" t="s">
+        <v>609</v>
+      </c>
+      <c r="I77" t="s">
+        <v>636</v>
+      </c>
+      <c r="J77" t="s">
         <v>355</v>
       </c>
-      <c r="I77" t="s">
+      <c r="K77" t="s">
         <v>65</v>
       </c>
-      <c r="J77" t="s">
+      <c r="L77" t="s">
         <v>218</v>
       </c>
-      <c r="K77" t="s">
+      <c r="M77" t="s">
         <v>364</v>
       </c>
-      <c r="L77" t="s">
+      <c r="N77" t="s">
         <v>416</v>
       </c>
-      <c r="M77" t="s">
+      <c r="O77" t="s">
         <v>438</v>
       </c>
-      <c r="N77" t="s">
+      <c r="P77" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>60</v>
       </c>
@@ -5499,28 +6167,34 @@
         <v>273</v>
       </c>
       <c r="H78" t="s">
+        <v>610</v>
+      </c>
+      <c r="I78" t="s">
+        <v>637</v>
+      </c>
+      <c r="J78" t="s">
         <v>356</v>
       </c>
-      <c r="I78" t="s">
+      <c r="K78" t="s">
         <v>66</v>
       </c>
-      <c r="J78" t="s">
+      <c r="L78" t="s">
         <v>219</v>
       </c>
-      <c r="K78" t="s">
+      <c r="M78" t="s">
         <v>365</v>
       </c>
-      <c r="L78" t="s">
+      <c r="N78" t="s">
         <v>417</v>
       </c>
-      <c r="M78" t="s">
+      <c r="O78" t="s">
         <v>439</v>
       </c>
-      <c r="N78" t="s">
+      <c r="P78" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>24</v>
       </c>
@@ -5543,28 +6217,34 @@
         <v>525</v>
       </c>
       <c r="H79" t="s">
+        <v>611</v>
+      </c>
+      <c r="I79" t="s">
+        <v>274</v>
+      </c>
+      <c r="J79" t="s">
         <v>518</v>
       </c>
-      <c r="I79" t="s">
+      <c r="K79" t="s">
         <v>295</v>
       </c>
-      <c r="J79" t="s">
+      <c r="L79" t="s">
         <v>534</v>
       </c>
-      <c r="K79" t="s">
+      <c r="M79" t="s">
         <v>41</v>
       </c>
-      <c r="L79" t="s">
+      <c r="N79" t="s">
         <v>274</v>
       </c>
-      <c r="M79" t="s">
+      <c r="O79" t="s">
         <v>30</v>
       </c>
-      <c r="N79" t="s">
+      <c r="P79" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>36</v>
       </c>
@@ -5587,28 +6267,34 @@
         <v>75</v>
       </c>
       <c r="H80" t="s">
+        <v>462</v>
+      </c>
+      <c r="I80" t="s">
+        <v>373</v>
+      </c>
+      <c r="J80" t="s">
         <v>519</v>
       </c>
-      <c r="I80" t="s">
+      <c r="K80" t="s">
         <v>254</v>
       </c>
-      <c r="J80" t="s">
+      <c r="L80" t="s">
         <v>535</v>
       </c>
-      <c r="K80" t="s">
+      <c r="M80" t="s">
         <v>491</v>
       </c>
-      <c r="L80" t="s">
+      <c r="N80" t="s">
         <v>242</v>
       </c>
-      <c r="M80" t="s">
+      <c r="O80" t="s">
         <v>486</v>
       </c>
-      <c r="N80" t="s">
+      <c r="P80" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>48</v>
       </c>
@@ -5631,28 +6317,34 @@
         <v>496</v>
       </c>
       <c r="H81" t="s">
+        <v>612</v>
+      </c>
+      <c r="I81" t="s">
+        <v>553</v>
+      </c>
+      <c r="J81" t="s">
         <v>437</v>
       </c>
-      <c r="I81" t="s">
+      <c r="K81" t="s">
         <v>530</v>
       </c>
-      <c r="J81" t="s">
+      <c r="L81" t="s">
         <v>392</v>
       </c>
-      <c r="K81" t="s">
+      <c r="M81" t="s">
         <v>492</v>
       </c>
-      <c r="L81" t="s">
+      <c r="N81" t="s">
         <v>500</v>
       </c>
-      <c r="M81" t="s">
+      <c r="O81" t="s">
         <v>146</v>
       </c>
-      <c r="N81" t="s">
+      <c r="P81" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>60</v>
       </c>
@@ -5675,28 +6367,34 @@
         <v>189</v>
       </c>
       <c r="H82" t="s">
+        <v>613</v>
+      </c>
+      <c r="I82" t="s">
+        <v>584</v>
+      </c>
+      <c r="J82" t="s">
         <v>333</v>
       </c>
-      <c r="I82" t="s">
+      <c r="K82" t="s">
         <v>531</v>
       </c>
-      <c r="J82" t="s">
+      <c r="L82" t="s">
         <v>32</v>
       </c>
-      <c r="K82" t="s">
+      <c r="M82" t="s">
         <v>493</v>
       </c>
-      <c r="L82" t="s">
+      <c r="N82" t="s">
         <v>501</v>
       </c>
-      <c r="M82" t="s">
+      <c r="O82" t="s">
         <v>56</v>
       </c>
-      <c r="N82" t="s">
+      <c r="P82" t="s">
         <v>547</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>24</v>
       </c>
@@ -5719,28 +6417,34 @@
         <v>565</v>
       </c>
       <c r="H83" t="s">
+        <v>614</v>
+      </c>
+      <c r="I83" t="s">
+        <v>159</v>
+      </c>
+      <c r="J83" t="s">
         <v>520</v>
       </c>
-      <c r="I83" t="s">
+      <c r="K83" t="s">
         <v>532</v>
       </c>
-      <c r="J83" t="s">
+      <c r="L83" t="s">
         <v>378</v>
       </c>
-      <c r="K83" t="s">
+      <c r="M83" t="s">
         <v>494</v>
       </c>
-      <c r="L83" t="s">
+      <c r="N83" t="s">
         <v>502</v>
       </c>
-      <c r="M83" t="s">
+      <c r="O83" t="s">
         <v>388</v>
       </c>
-      <c r="N83" t="s">
+      <c r="P83" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>96</v>
       </c>
@@ -5763,28 +6467,34 @@
         <v>380</v>
       </c>
       <c r="H84" t="s">
+        <v>216</v>
+      </c>
+      <c r="I84" t="s">
+        <v>558</v>
+      </c>
+      <c r="J84" t="s">
         <v>521</v>
       </c>
-      <c r="I84" t="s">
+      <c r="K84" t="s">
         <v>533</v>
       </c>
-      <c r="J84" t="s">
+      <c r="L84" t="s">
         <v>486</v>
       </c>
-      <c r="K84" t="s">
+      <c r="M84" t="s">
         <v>406</v>
       </c>
-      <c r="L84" t="s">
+      <c r="N84" t="s">
         <v>503</v>
       </c>
-      <c r="M84" t="s">
+      <c r="O84" t="s">
         <v>487</v>
       </c>
-      <c r="N84" t="s">
+      <c r="P84" t="s">
         <v>549</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>192</v>
       </c>
@@ -5807,28 +6517,34 @@
         <v>33</v>
       </c>
       <c r="H85" t="s">
+        <v>615</v>
+      </c>
+      <c r="I85" t="s">
+        <v>86</v>
+      </c>
+      <c r="J85" t="s">
         <v>522</v>
       </c>
-      <c r="I85" t="s">
+      <c r="K85" t="s">
         <v>169</v>
       </c>
-      <c r="J85" t="s">
+      <c r="L85" t="s">
         <v>508</v>
       </c>
-      <c r="K85" t="s">
+      <c r="M85" t="s">
         <v>385</v>
       </c>
-      <c r="L85" t="s">
+      <c r="N85" t="s">
         <v>305</v>
       </c>
-      <c r="M85" t="s">
+      <c r="O85" t="s">
         <v>77</v>
       </c>
-      <c r="N85" t="s">
+      <c r="P85" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>336</v>
       </c>
@@ -5851,28 +6567,34 @@
         <v>566</v>
       </c>
       <c r="H86" t="s">
+        <v>519</v>
+      </c>
+      <c r="I86" t="s">
+        <v>141</v>
+      </c>
+      <c r="J86" t="s">
         <v>523</v>
       </c>
-      <c r="I86" t="s">
+      <c r="K86" t="s">
         <v>229</v>
       </c>
-      <c r="J86" t="s">
+      <c r="L86" t="s">
         <v>390</v>
       </c>
-      <c r="K86" t="s">
+      <c r="M86" t="s">
         <v>212</v>
       </c>
-      <c r="L86" t="s">
+      <c r="N86" t="s">
         <v>504</v>
       </c>
-      <c r="M86" t="s">
+      <c r="O86" t="s">
         <v>138</v>
       </c>
-      <c r="N86" t="s">
+      <c r="P86" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>720</v>
       </c>
@@ -5895,24 +6617,30 @@
         <v>173</v>
       </c>
       <c r="H87" t="s">
+        <v>616</v>
+      </c>
+      <c r="I87" t="s">
+        <v>638</v>
+      </c>
+      <c r="J87" t="s">
         <v>524</v>
       </c>
-      <c r="I87" t="s">
+      <c r="K87" t="s">
         <v>45</v>
       </c>
-      <c r="J87" t="s">
+      <c r="L87" t="s">
         <v>70</v>
       </c>
-      <c r="K87" t="s">
+      <c r="M87" t="s">
         <v>495</v>
       </c>
-      <c r="L87" t="s">
+      <c r="N87" t="s">
         <v>505</v>
       </c>
-      <c r="M87" t="s">
+      <c r="O87" t="s">
         <v>162</v>
       </c>
-      <c r="N87" t="s">
+      <c r="P87" t="s">
         <v>552</v>
       </c>
     </row>

</xml_diff>